<commit_message>
updates excel, PECore Signed-off-by: Iulia Chereja <chereja_iulia@yahoo.com>
</commit_message>
<xml_diff>
--- a/src/PELib/gates.xlsx
+++ b/src/PELib/gates.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC165D19-50D3-4B50-8586-8FBD5F7DAC14}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A7659FB-FE7E-484F-8E2D-EC8B8014E84A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="19560" windowHeight="8130" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="17" r:id="rId1"/>
@@ -19,10 +19,10 @@
     <sheet name="wsclibx2" sheetId="5" r:id="rId9"/>
     <sheet name="vgalibx2" sheetId="6" r:id="rId10"/>
     <sheet name="rgalibx2" sheetId="7" r:id="rId11"/>
-    <sheet name="74ac" sheetId="9" r:id="rId12"/>
-    <sheet name="74act" sheetId="10" r:id="rId13"/>
-    <sheet name="74hc" sheetId="11" r:id="rId14"/>
-    <sheet name="74hct" sheetId="12" r:id="rId15"/>
+    <sheet name="ac" sheetId="19" r:id="rId12"/>
+    <sheet name="act" sheetId="20" r:id="rId13"/>
+    <sheet name="hc" sheetId="21" r:id="rId14"/>
+    <sheet name="hct" sheetId="22" r:id="rId15"/>
     <sheet name="cmos" sheetId="13" r:id="rId16"/>
   </sheets>
   <definedNames>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="68">
   <si>
     <t>Type Gate</t>
   </si>
@@ -89,57 +89,6 @@
   </si>
   <si>
     <t>Generic 0.13 um typical timing (ps &amp; ps/fF)</t>
-  </si>
-  <si>
-    <t>AND3</t>
-  </si>
-  <si>
-    <t>AND2</t>
-  </si>
-  <si>
-    <t>AND4</t>
-  </si>
-  <si>
-    <t>BUFFER NON-INV</t>
-  </si>
-  <si>
-    <t>INVERTER</t>
-  </si>
-  <si>
-    <t>MUX2:1</t>
-  </si>
-  <si>
-    <t>NAND2</t>
-  </si>
-  <si>
-    <t>NAND3</t>
-  </si>
-  <si>
-    <t>NAND4</t>
-  </si>
-  <si>
-    <t>NOR2</t>
-  </si>
-  <si>
-    <t>NOR3</t>
-  </si>
-  <si>
-    <t>NOR4</t>
-  </si>
-  <si>
-    <t>NXOR</t>
-  </si>
-  <si>
-    <t>OR2</t>
-  </si>
-  <si>
-    <t>OR3</t>
-  </si>
-  <si>
-    <t>OR4</t>
-  </si>
-  <si>
-    <t>XOR</t>
   </si>
   <si>
     <t>Icc[nA]</t>
@@ -193,18 +142,6 @@
     <t>Area=H*W [um*um]</t>
   </si>
   <si>
-    <t>MUX4:1</t>
-  </si>
-  <si>
-    <t>NUM163</t>
-  </si>
-  <si>
-    <t>TRISTATE BUFFER</t>
-  </si>
-  <si>
-    <t>DFF(rising edge)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Parametri</t>
   </si>
   <si>
@@ -227,6 +164,84 @@
   </si>
   <si>
     <t>Cin[pF]</t>
+  </si>
+  <si>
+    <t>tristate_buffer</t>
+  </si>
+  <si>
+    <t>buffer_non_inv</t>
+  </si>
+  <si>
+    <t>inverter</t>
+  </si>
+  <si>
+    <t>and2</t>
+  </si>
+  <si>
+    <t>and3</t>
+  </si>
+  <si>
+    <t>and4</t>
+  </si>
+  <si>
+    <t>or2</t>
+  </si>
+  <si>
+    <t>or3</t>
+  </si>
+  <si>
+    <t>or4</t>
+  </si>
+  <si>
+    <t>nand2</t>
+  </si>
+  <si>
+    <t>anad3</t>
+  </si>
+  <si>
+    <t>nand4</t>
+  </si>
+  <si>
+    <t>nor2</t>
+  </si>
+  <si>
+    <t>nor3</t>
+  </si>
+  <si>
+    <t>nor4</t>
+  </si>
+  <si>
+    <t>xor</t>
+  </si>
+  <si>
+    <t>xnor</t>
+  </si>
+  <si>
+    <t>mux2:1</t>
+  </si>
+  <si>
+    <t>mux4:1</t>
+  </si>
+  <si>
+    <t>num163</t>
+  </si>
+  <si>
+    <t>dff_rising_edge</t>
+  </si>
+  <si>
+    <t>xor2</t>
+  </si>
+  <si>
+    <t>xnor2</t>
+  </si>
+  <si>
+    <t>nand3</t>
+  </si>
+  <si>
+    <t>mux2</t>
+  </si>
+  <si>
+    <t>mux4</t>
   </si>
 </sst>
 </file>
@@ -377,7 +392,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,6 +407,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A982735-C675-46F5-98D6-7FE0AAC31E76}">
   <dimension ref="A8:A28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A28"/>
+    <sheetView topLeftCell="A7" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,132 +701,133 @@
   <sheetData>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>ssxlibx2!A8&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q8,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q8, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q8,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q8, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q8, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q8, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q8, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q8, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q8, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q8, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q8, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q8,"0.00E+00")&amp;")"</f>
-        <v>TRISTATE BUFFER  =&gt;  ( ssxlib =&gt; 0.000E+00  , sxlib =&gt; 0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A8 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q8,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q8,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q8,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q8, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q8, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q8, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q8, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q8, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q8, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q8, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q8, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q8,"0.00E+00")&amp;"),"</f>
+        <v>tristate_buffer =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>ssxlibx2!A9&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q9,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q9, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q9,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q9, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q9, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q9, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q9, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q9, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q9, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q9, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q9, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q9,"0.00E+00")&amp;")"</f>
-        <v>BUFFER NON-INV  =&gt;  ( ssxlib =&gt; 012E+00  , sxlib =&gt; 012E+00 , vxlib =&gt; 012E+00 , vsclib =&gt; 007E+00 , wsclib =&gt; 008E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A9 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q9,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q9,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q9,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q9, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q9, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q9, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q9, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q9, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q9, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q9, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q9, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q9,"0.00E+00")&amp;"),"</f>
+        <v>buffer_non_inv =&gt;( ssxlib =&gt; 012E+00, sxlib =&gt;  012E+00 , vxlib =&gt; 012E+00 , vsclib =&gt; 007E+00 , wsclib =&gt; 008E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>ssxlibx2!A10&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q10,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q10, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q10,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q10, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q10, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q10, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q10, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q10, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q10, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q10, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q10, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q10,"0.00E+00")&amp;")"</f>
-        <v>INVERTER  =&gt;  ( ssxlib =&gt; 009E+00  , sxlib =&gt; 009E+00 , vxlib =&gt; 009E+00 , vsclib =&gt; 005E+00 , wsclib =&gt; 006E+00 , vgalib =&gt; 009E+00 , rgalib =&gt; 009E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A10 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q10,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q10,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q10,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q10, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q10, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q10, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q10, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q10, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q10, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q10, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q10, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q10,"0.00E+00")&amp;"),"</f>
+        <v>inverter =&gt;( ssxlib =&gt; 009E+00, sxlib =&gt;  009E+00 , vxlib =&gt; 009E+00 , vsclib =&gt; 005E+00 , wsclib =&gt; 006E+00 , vgalib =&gt; 009E+00 , rgalib =&gt; 009E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>ssxlibx2!A11&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q11,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q11, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q11,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q11, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q11, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q11, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q11, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q11, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q11, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q11, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q11, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q11,"0.00E+00")&amp;")"</f>
-        <v>AND2  =&gt;  ( ssxlib =&gt; 015E+00  , sxlib =&gt; 015E+00 , vxlib =&gt; 015E+00 , vsclib =&gt; 009E+00 , wsclib =&gt; 010E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A11 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q11,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q11,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q11,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q11, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q11, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q11, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q11, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q11, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q11, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q11, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q11, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q11,"0.00E+00")&amp;"),"</f>
+        <v>and2 =&gt;( ssxlib =&gt; 015E+00, sxlib =&gt;  015E+00 , vxlib =&gt; 015E+00 , vsclib =&gt; 009E+00 , wsclib =&gt; 010E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>ssxlibx2!A12&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q12,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q12, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q12,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q12, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q12, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q12, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q12, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q12, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q12, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q12, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q12, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q12,"0.00E+00")&amp;")"</f>
-        <v>AND3  =&gt;  ( ssxlib =&gt; 018E+00  , sxlib =&gt; 018E+00 , vxlib =&gt; 018E+00 , vsclib =&gt; 012E+00 , wsclib =&gt; 014E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A12 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q12,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q12,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q12,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q12, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q12, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q12, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q12, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q12, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q12, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q12, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q12, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q12,"0.00E+00")&amp;"),"</f>
+        <v>and3 =&gt;( ssxlib =&gt; 018E+00, sxlib =&gt;  018E+00 , vxlib =&gt; 018E+00 , vsclib =&gt; 012E+00 , wsclib =&gt; 014E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>ssxlibx2!A13&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q13,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q13, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q13,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q13, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q13, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q13, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q13, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q13, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q13, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q13, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q13, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q13,"0.00E+00")&amp;")"</f>
-        <v>AND4  =&gt;  ( ssxlib =&gt; 021E+00  , sxlib =&gt; 021E+00 , vxlib =&gt; 021E+00 , vsclib =&gt; 014E+00 , wsclib =&gt; 015E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A13 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q13,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q13,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q13,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q13, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q13, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q13, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q13, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q13, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q13, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q13, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q13, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q13,"0.00E+00")&amp;"),"</f>
+        <v>and4 =&gt;( ssxlib =&gt; 021E+00, sxlib =&gt;  021E+00 , vxlib =&gt; 021E+00 , vsclib =&gt; 014E+00 , wsclib =&gt; 015E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>ssxlibx2!A14&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q14,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q14, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q14,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q14, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q14, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q14, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q14, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q14, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q14, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q14, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q14, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q14,"0.00E+00")&amp;")"</f>
-        <v>OR2  =&gt;  ( ssxlib =&gt; 015E+00  , sxlib =&gt; 015E+00 , vxlib =&gt; 015E+00 , vsclib =&gt; 009E+00 , wsclib =&gt; 010E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A14 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q14,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q14,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q14,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q14, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q14, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q14, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q14, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q14, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q14, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q14, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q14, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q14,"0.00E+00")&amp;"),"</f>
+        <v>or2 =&gt;( ssxlib =&gt; 015E+00, sxlib =&gt;  015E+00 , vxlib =&gt; 015E+00 , vsclib =&gt; 009E+00 , wsclib =&gt; 010E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>ssxlibx2!A15&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q15,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q15, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q15,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q15, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q15, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q15, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q15, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q15, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q15, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q15, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q15, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q15,"0.00E+00")&amp;")"</f>
-        <v>OR3  =&gt;  ( ssxlib =&gt; 018E+00  , sxlib =&gt; 018E+00 , vxlib =&gt; 018E+00 , vsclib =&gt; 016E+00 , wsclib =&gt; 017E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A15 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q15,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q15,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q15,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q15, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q15, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q15, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q15, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q15, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q15, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q15, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q15, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q15,"0.00E+00")&amp;"),"</f>
+        <v>or3 =&gt;( ssxlib =&gt; 018E+00, sxlib =&gt;  018E+00 , vxlib =&gt; 018E+00 , vsclib =&gt; 016E+00 , wsclib =&gt; 017E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>ssxlibx2!A16&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q16,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q16, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q16,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q16, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q16, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q16, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q16, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q16, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q16, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q16, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q16, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q16,"0.00E+00")&amp;")"</f>
-        <v>OR4  =&gt;  ( ssxlib =&gt; 021E+00  , sxlib =&gt; 021E+00 , vxlib =&gt; 024E+00 , vsclib =&gt; 019E+00 , wsclib =&gt; 021E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A16 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q16,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q16,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q16,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q16, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q16, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q16, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q16, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q16, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q16, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q16, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q16, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q16,"0.00E+00")&amp;"),"</f>
+        <v>or4 =&gt;( ssxlib =&gt; 021E+00, sxlib =&gt;  021E+00 , vxlib =&gt; 024E+00 , vsclib =&gt; 019E+00 , wsclib =&gt; 021E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>ssxlibx2!A17&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q17,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q17, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q17,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q17, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q17, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q17, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q17, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q17, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q17, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q17, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q17, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q17,"0.00E+00")&amp;")"</f>
-        <v>NAND2  =&gt;  ( ssxlib =&gt; 012E+00  , sxlib =&gt; 012E+00 , vxlib =&gt; 012E+00 , vsclib =&gt; 007E+00 , wsclib =&gt; 008E+00 , vgalib =&gt; 009E+00 , rgalib =&gt; 009E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A17 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q17,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q17,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q17,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q17, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q17, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q17, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q17, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q17, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q17, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q17, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q17, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q17,"0.00E+00")&amp;"),"</f>
+        <v>nand2 =&gt;( ssxlib =&gt; 012E+00, sxlib =&gt;  012E+00 , vxlib =&gt; 012E+00 , vsclib =&gt; 007E+00 , wsclib =&gt; 008E+00 , vgalib =&gt; 009E+00 , rgalib =&gt; 009E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>ssxlibx2!A18&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q18,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q18, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q18,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q18, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q18, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q18, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q18, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q18, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q18, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q18, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q18, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q18,"0.00E+00")&amp;")"</f>
-        <v>NAND3  =&gt;  ( ssxlib =&gt; 015E+00  , sxlib =&gt; 015E+00 , vxlib =&gt; 015E+00 , vsclib =&gt; 014E+00 , wsclib =&gt; 015E+00 , vgalib =&gt; 017E+00 , rgalib =&gt; 017E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A18 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q18,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q18,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q18,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q18, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q18, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q18, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q18, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q18, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q18, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q18, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q18, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q18,"0.00E+00")&amp;"),"</f>
+        <v>nand3 =&gt;( ssxlib =&gt; 015E+00, sxlib =&gt;  015E+00 , vxlib =&gt; 015E+00 , vsclib =&gt; 014E+00 , wsclib =&gt; 015E+00 , vgalib =&gt; 017E+00 , rgalib =&gt; 017E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>ssxlibx2!A19&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q19,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q19, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q19,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q19, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q19, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q19, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q19, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q19, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q19, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q19, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q19, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q19,"0.00E+00")&amp;")"</f>
-        <v>NAND4  =&gt;  ( ssxlib =&gt; 018E+00  , sxlib =&gt; 018E+00 , vxlib =&gt; 027E+00 , vsclib =&gt; 017E+00 , wsclib =&gt; 019E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A19 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q19,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q19,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q19,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q19, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q19, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q19, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q19, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q19, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q19, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q19, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q19, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q19,"0.00E+00")&amp;"),"</f>
+        <v>nand4 =&gt;( ssxlib =&gt; 018E+00, sxlib =&gt;  018E+00 , vxlib =&gt; 027E+00 , vsclib =&gt; 017E+00 , wsclib =&gt; 019E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>ssxlibx2!A20&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q20,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q20, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q20,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q20, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q20, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q20, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q20, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q20, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q20, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q20, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q20, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q20,"0.00E+00")&amp;")"</f>
-        <v>NOR2  =&gt;  ( ssxlib =&gt; 012E+00  , sxlib =&gt; 012E+00 , vxlib =&gt; 018E+00 , vsclib =&gt; 010E+00 , wsclib =&gt; 012E+00 , vgalib =&gt; 017E+00 , rgalib =&gt; 017E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A20 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q20,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q20,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q20,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q20, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q20, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q20, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q20, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q20, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q20, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q20, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q20, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q20,"0.00E+00")&amp;"),"</f>
+        <v>nor2 =&gt;( ssxlib =&gt; 012E+00, sxlib =&gt;  012E+00 , vxlib =&gt; 018E+00 , vsclib =&gt; 010E+00 , wsclib =&gt; 012E+00 , vgalib =&gt; 017E+00 , rgalib =&gt; 017E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>ssxlibx2!A21&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q21,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q21, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q21,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q21, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q21, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q21, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q21, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q21, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q21, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q21, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q21, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q21,"0.00E+00")&amp;")"</f>
-        <v>NOR3  =&gt;  ( ssxlib =&gt; 015E+00  , sxlib =&gt; 015E+00 , vxlib =&gt; 021E+00 , vsclib =&gt; 019E+00 , wsclib =&gt; 021E+00 , vgalib =&gt; 026E+00 , rgalib =&gt; 026E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A21 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q21,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q21,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q21,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q21, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q21, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q21, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q21, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q21, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q21, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q21, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q21, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q21,"0.00E+00")&amp;"),"</f>
+        <v>nor3 =&gt;( ssxlib =&gt; 015E+00, sxlib =&gt;  015E+00 , vxlib =&gt; 021E+00 , vsclib =&gt; 019E+00 , wsclib =&gt; 021E+00 , vgalib =&gt; 026E+00 , rgalib =&gt; 026E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>ssxlibx2!A22&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q22,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q22, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q22,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q22, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q22, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q22, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q22, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q22, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q22, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q22, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q22, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q22,"0.00E+00")&amp;")"</f>
-        <v>NOR4  =&gt;  ( ssxlib =&gt; 018E+00  , sxlib =&gt; 018E+00 , vxlib =&gt; 027E+00 , vsclib =&gt; 024E+00 , wsclib =&gt; 027E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A22 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q22,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q22,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q22,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q22, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q22, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q22, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q22, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q22, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q22, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q22, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q22, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q22,"0.00E+00")&amp;"),"</f>
+        <v>nor4 =&gt;( ssxlib =&gt; 018E+00, sxlib =&gt;  018E+00 , vxlib =&gt; 027E+00 , vsclib =&gt; 024E+00 , wsclib =&gt; 027E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>ssxlibx2!A23&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q23,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q23, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q23,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q23, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q23, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q23, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q23, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q23, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q23, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q23, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q23, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q23,"0.00E+00")&amp;")"</f>
-        <v>XOR  =&gt;  ( ssxlib =&gt; 027E+00  , sxlib =&gt; 027E+00 , vxlib =&gt; 021E+00 , vsclib =&gt; 024E+00 , wsclib =&gt; 027E+00 , vgalib =&gt; 026E+00 , rgalib =&gt; 026E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A23 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q23,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q23,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q23,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q23, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q23, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q23, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q23, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q23, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q23, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q23, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q23, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q23,"0.00E+00")&amp;"),"</f>
+        <v>xor2 =&gt;( ssxlib =&gt; 027E+00, sxlib =&gt;  027E+00 , vxlib =&gt; 021E+00 , vsclib =&gt; 024E+00 , wsclib =&gt; 027E+00 , vgalib =&gt; 026E+00 , rgalib =&gt; 026E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>ssxlibx2!A24&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q24,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q24, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q24,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q24, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q24, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q24, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q24, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q24, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q24, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q24, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q24, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q24,"0.00E+00")&amp;")"</f>
-        <v>NXOR  =&gt;  ( ssxlib =&gt; 027E+00  , sxlib =&gt; 027E+00 , vxlib =&gt; 021E+00 , vsclib =&gt; 023E+00 , wsclib =&gt; 025E+00 , vgalib =&gt; 026E+00 , rgalib =&gt; 026E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A24 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q24,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q24,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q24,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q24, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q24, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q24, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q24, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q24, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q24, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q24, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q24, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q24,"0.00E+00")&amp;"),"</f>
+        <v>xnor2 =&gt;( ssxlib =&gt; 027E+00, sxlib =&gt;  027E+00 , vxlib =&gt; 021E+00 , vsclib =&gt; 023E+00 , wsclib =&gt; 025E+00 , vgalib =&gt; 026E+00 , rgalib =&gt; 026E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>ssxlibx2!A25&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q25,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q25, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q25,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q25, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q25, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q25, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q25, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q25, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q25, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q25, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q25, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q25,"0.00E+00")&amp;")"</f>
-        <v>MUX2:1  =&gt;  ( ssxlib =&gt; 027E+00  , sxlib =&gt; 027E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 015E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A25 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q25,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q25,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q25,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q25, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q25, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q25, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q25, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q25, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q25, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q25, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q25, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q25,"0.00E+00")&amp;"),"</f>
+        <v>mux2 =&gt;( ssxlib =&gt; 027E+00, sxlib =&gt;  027E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 015E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>ssxlibx2!A26&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q26,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q26, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q26,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q26, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q26, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q26, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q26, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q26, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q26, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q26, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q26, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q26,"0.00E+00")&amp;")"</f>
-        <v>MUX4:1  =&gt;  ( ssxlib =&gt; 0.000E+00  , sxlib =&gt; 0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A26 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q26,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q26,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q26,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q26, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q26, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q26, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q26, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q26, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q26, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q26, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q26, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q26,"0.00E+00")&amp;"),"</f>
+        <v>mux4 =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>ssxlibx2!A27&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q27,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q27, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q27,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q27, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q27, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q27, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q27, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q27, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q27, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q27, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q27, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q27,"0.00E+00")&amp;")"</f>
-        <v>NUM163  =&gt;  ( ssxlib =&gt; 0.000E+00  , sxlib =&gt; 0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A27 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q27,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q27,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q27,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q27, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q27, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q27, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q27, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q27, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q27, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q27, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q27, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q27,"0.00E+00")&amp;"),"</f>
+        <v>num163 =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f>ssxlibx2!A28&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q28,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!Q28, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q28,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q28, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q28, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q28, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q28, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!Q28, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!Q28, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!Q28, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!Q28, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q28,"0.00E+00")&amp;")"</f>
-        <v>DFF(rising edge)  =&gt;  ( ssxlib =&gt; 0.000E+00  , sxlib =&gt; 0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 044E+00 , wsclib =&gt; 035E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A28 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q28,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q28,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q28,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q28, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q28, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q28, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q28, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q28, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q28, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q28, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q28, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q28,"0.00E+00")&amp;"),"</f>
+        <v>dff_rising_edge =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 044E+00 , wsclib =&gt; 035E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -819,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235D5E8D-EE9A-4F3B-A6F6-ECFF36D9C647}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7:Q28"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,16 +850,16 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -851,13 +867,13 @@
         <v>1.2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -866,49 +882,49 @@
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="27" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="24" t="s">
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="23"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="22"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
@@ -930,7 +946,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>13</v>
@@ -945,27 +961,27 @@
         <v>12</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B8" s="14">
         <v>0</v>
@@ -1024,7 +1040,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B9" s="14">
         <v>0</v>
@@ -1083,7 +1099,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>1.3</v>
@@ -1142,7 +1158,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B11" s="14">
         <v>0</v>
@@ -1201,7 +1217,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B12" s="14">
         <v>0</v>
@@ -1260,7 +1276,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B13" s="14">
         <v>0</v>
@@ -1319,7 +1335,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B14" s="14">
         <v>0</v>
@@ -1378,7 +1394,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B15" s="14">
         <v>0</v>
@@ -1437,7 +1453,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B16" s="14">
         <v>0</v>
@@ -1496,7 +1512,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>1.3</v>
@@ -1555,7 +1571,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B18">
         <v>2.7</v>
@@ -1614,7 +1630,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1673,7 +1689,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B20">
         <v>2.7</v>
@@ -1732,7 +1748,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -1791,7 +1807,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1850,7 +1866,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -1909,7 +1925,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -1968,7 +1984,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -2027,7 +2043,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -2086,7 +2102,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -2145,7 +2161,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -2220,8 +2236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F4B815-9755-4EA2-9594-76C4C8E69D25}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,16 +2249,16 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2250,13 +2266,13 @@
         <v>1.2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -2265,49 +2281,49 @@
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="27" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="24" t="s">
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="23"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="22"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
@@ -2329,7 +2345,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>13</v>
@@ -2344,27 +2360,27 @@
         <v>12</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B8" s="14">
         <v>0</v>
@@ -2423,7 +2439,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B9" s="14">
         <v>0</v>
@@ -2482,7 +2498,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>1.3</v>
@@ -2541,7 +2557,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B11" s="14">
         <v>0</v>
@@ -2600,7 +2616,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B12" s="14">
         <v>0</v>
@@ -2659,7 +2675,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B13" s="14">
         <v>0</v>
@@ -2718,7 +2734,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B14" s="14">
         <v>0</v>
@@ -2777,7 +2793,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B15" s="14">
         <v>0</v>
@@ -2836,7 +2852,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B16" s="14">
         <v>0</v>
@@ -2895,7 +2911,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>1.3</v>
@@ -2954,7 +2970,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B18">
         <v>2.7</v>
@@ -3013,7 +3029,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -3072,7 +3088,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B20">
         <v>2.7</v>
@@ -3131,7 +3147,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -3190,7 +3206,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -3249,7 +3265,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -3308,7 +3324,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -3367,7 +3383,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -3426,7 +3442,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -3485,7 +3501,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -3544,7 +3560,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -3616,11 +3632,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7E11D19-7519-4210-8FD0-8D22A973D5D9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FB08D7-F942-4778-BD1F-B00B32A28B6E}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3631,10 +3647,10 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3642,18 +3658,18 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L6" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
+      <c r="L6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
       <c r="Q6" s="18" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3661,21 +3677,21 @@
         <v>0</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="L8" s="10">
         <v>2</v>
@@ -3692,7 +3708,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="L9" s="10">
         <v>0</v>
@@ -3709,7 +3725,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="L10" s="10">
         <v>2</v>
@@ -3726,7 +3742,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="L11" s="10">
         <v>2</v>
@@ -3743,7 +3759,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="L12" s="10">
         <v>0</v>
@@ -3760,7 +3776,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="L13" s="10">
         <v>0</v>
@@ -3777,7 +3793,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="L14" s="10">
         <v>2</v>
@@ -3794,7 +3810,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="L15" s="10">
         <v>0</v>
@@ -3811,7 +3827,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="L16" s="10">
         <v>0</v>
@@ -3828,7 +3844,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="L17" s="10">
         <v>2</v>
@@ -3845,7 +3861,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="L18" s="10">
         <v>2</v>
@@ -3862,7 +3878,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="L19" s="10">
         <v>2</v>
@@ -3879,7 +3895,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="L20" s="10">
         <v>2</v>
@@ -3896,7 +3912,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="L21" s="10">
         <v>0</v>
@@ -3913,7 +3929,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="L22" s="10">
         <v>0</v>
@@ -3930,7 +3946,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="L23" s="10">
         <v>2</v>
@@ -3947,7 +3963,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="L24" s="10">
         <v>0</v>
@@ -3964,7 +3980,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="L25" s="10">
         <v>0</v>
@@ -3981,7 +3997,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="L26" s="10">
         <v>0</v>
@@ -3998,7 +4014,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="L27" s="10">
         <v>0</v>
@@ -4015,7 +4031,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L28" s="10">
         <v>0</v>
@@ -4035,16 +4051,15 @@
     <mergeCell ref="L6:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB0495A-EBF4-462D-A153-3F78DFE4DE22}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3D0F2B-832D-4300-97D5-DDEB6D07CF40}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4055,10 +4070,10 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4066,18 +4081,18 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L6" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
+      <c r="L6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
       <c r="Q6" s="18" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4085,21 +4100,21 @@
         <v>0</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="L8" s="10">
         <v>8</v>
@@ -4116,7 +4131,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="L9" s="10">
         <v>0</v>
@@ -4133,7 +4148,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="L10" s="10">
         <v>4</v>
@@ -4150,7 +4165,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="L11" s="10">
         <v>4</v>
@@ -4167,7 +4182,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="L12" s="10">
         <v>0</v>
@@ -4184,7 +4199,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="L13" s="10">
         <v>0</v>
@@ -4201,7 +4216,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="L14" s="10">
         <v>4</v>
@@ -4218,7 +4233,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="L15" s="10">
         <v>0</v>
@@ -4235,7 +4250,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="L16" s="10">
         <v>0</v>
@@ -4252,7 +4267,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="L17" s="10">
         <v>2</v>
@@ -4269,7 +4284,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="L18" s="10">
         <v>4</v>
@@ -4286,7 +4301,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="L19" s="10">
         <v>4</v>
@@ -4303,7 +4318,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="L20" s="10">
         <v>4</v>
@@ -4320,7 +4335,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="L21" s="10">
         <v>0</v>
@@ -4337,7 +4352,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="L22" s="10">
         <v>0</v>
@@ -4354,7 +4369,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="L23" s="10">
         <v>2</v>
@@ -4371,7 +4386,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="L24" s="10">
         <v>0</v>
@@ -4388,7 +4403,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="L25" s="10">
         <v>0</v>
@@ -4405,7 +4420,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="L26" s="10">
         <v>0</v>
@@ -4422,7 +4437,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="L27" s="10">
         <v>0</v>
@@ -4439,7 +4454,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L28" s="10">
         <v>0</v>
@@ -4463,11 +4478,11 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15CE1FF-162C-4241-B651-C05211996F02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F873900-F695-4C83-85AF-B7B87EDD7FCF}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4478,10 +4493,10 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4489,18 +4504,18 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L6" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
+      <c r="L6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
       <c r="Q6" s="18" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4508,21 +4523,21 @@
         <v>0</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="L8" s="10">
         <v>4</v>
@@ -4539,7 +4554,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="L9" s="10">
         <v>0</v>
@@ -4556,7 +4571,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="L10" s="10">
         <v>2</v>
@@ -4573,7 +4588,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="L11" s="10">
         <v>2</v>
@@ -4590,7 +4605,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="L12" s="10">
         <v>0</v>
@@ -4607,7 +4622,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="L13" s="10">
         <v>0</v>
@@ -4624,7 +4639,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="L14" s="10">
         <v>2</v>
@@ -4641,7 +4656,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="L15" s="10">
         <v>0</v>
@@ -4658,7 +4673,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="L16" s="10">
         <v>0</v>
@@ -4675,7 +4690,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="L17" s="10">
         <v>0</v>
@@ -4692,7 +4707,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="L18" s="10">
         <v>0</v>
@@ -4709,7 +4724,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="L19" s="10">
         <v>0</v>
@@ -4726,7 +4741,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="L20" s="10">
         <v>0</v>
@@ -4743,7 +4758,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="L21" s="10">
         <v>0</v>
@@ -4760,7 +4775,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="L22" s="10">
         <v>0</v>
@@ -4777,7 +4792,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="L23" s="10">
         <v>0</v>
@@ -4794,7 +4809,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="L24" s="10">
         <v>0</v>
@@ -4811,7 +4826,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="L25" s="10">
         <v>0</v>
@@ -4828,7 +4843,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="L26" s="10">
         <v>8</v>
@@ -4845,7 +4860,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="L27" s="10">
         <v>8</v>
@@ -4862,7 +4877,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L28" s="10">
         <v>0</v>
@@ -4886,11 +4901,11 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35F294C-61E7-4D48-90EC-5536A6423965}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E3FCF2-1EFF-46E6-81A7-08A9A539DC92}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4901,10 +4916,10 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4912,18 +4927,18 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L6" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
+      <c r="L6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
       <c r="Q6" s="18" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4931,21 +4946,21 @@
         <v>0</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="L8" s="10">
         <v>8</v>
@@ -4962,7 +4977,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="L9" s="10">
         <v>0</v>
@@ -4979,7 +4994,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="L10" s="10">
         <v>0</v>
@@ -4996,7 +5011,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="L11" s="10">
         <v>0</v>
@@ -5013,7 +5028,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="L12" s="10">
         <v>0</v>
@@ -5030,7 +5045,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="L13" s="10">
         <v>0</v>
@@ -5047,7 +5062,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="L14" s="10">
         <v>0</v>
@@ -5064,7 +5079,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="L15" s="10">
         <v>0</v>
@@ -5081,7 +5096,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="L16" s="10">
         <v>0</v>
@@ -5098,7 +5113,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="L17" s="10">
         <v>0</v>
@@ -5115,7 +5130,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="L18" s="10">
         <v>0</v>
@@ -5132,7 +5147,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="L19" s="10">
         <v>0</v>
@@ -5149,7 +5164,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="L20" s="10">
         <v>0</v>
@@ -5166,7 +5181,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="L21" s="10">
         <v>0</v>
@@ -5183,7 +5198,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="L22" s="10">
         <v>0</v>
@@ -5200,7 +5215,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="L23" s="10">
         <v>0</v>
@@ -5217,7 +5232,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="L24" s="10">
         <v>0</v>
@@ -5234,7 +5249,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="L25" s="10">
         <v>0</v>
@@ -5251,7 +5266,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="L26" s="10">
         <v>0</v>
@@ -5268,7 +5283,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="L27" s="10">
         <v>0</v>
@@ -5285,7 +5300,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L28" s="10">
         <v>0</v>
@@ -5312,8 +5327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DCB8990-16FC-4DA4-A64E-185EE2DC6D83}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5324,10 +5339,10 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5335,18 +5350,18 @@
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L6" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
+      <c r="L6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
       <c r="Q6" s="18" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5354,21 +5369,21 @@
         <v>0</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="Q7" s="19" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="L8" s="10">
         <v>0</v>
@@ -5385,7 +5400,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="L9" s="10">
         <v>0</v>
@@ -5402,7 +5417,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="L10" s="10">
         <v>10</v>
@@ -5419,7 +5434,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="L11" s="10">
         <v>4</v>
@@ -5436,7 +5451,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="L12" s="10">
         <v>10</v>
@@ -5453,7 +5468,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="L13" s="10">
         <v>10</v>
@@ -5470,7 +5485,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="L14" s="10">
         <v>4</v>
@@ -5487,7 +5502,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="L15" s="10">
         <v>10</v>
@@ -5504,7 +5519,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="L16" s="10">
         <v>250</v>
@@ -5521,7 +5536,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="L17" s="10">
         <v>4</v>
@@ -5538,7 +5553,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="L18" s="10">
         <v>4</v>
@@ -5555,7 +5570,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="L19" s="10">
         <v>5</v>
@@ -5572,7 +5587,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="L20" s="10">
         <v>4</v>
@@ -5589,7 +5604,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="L21" s="10">
         <v>5</v>
@@ -5606,7 +5621,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="L22" s="10">
         <v>5</v>
@@ -5623,7 +5638,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="L23" s="10">
         <v>50</v>
@@ -5640,7 +5655,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="L24" s="10">
         <v>100</v>
@@ -5657,7 +5672,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="L25" s="10">
         <v>0</v>
@@ -5674,7 +5689,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="L26" s="10">
         <v>0</v>
@@ -5691,7 +5706,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="L27" s="10">
         <v>0</v>
@@ -5708,7 +5723,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="L28" s="10">
         <v>0</v>
@@ -5735,8 +5750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD808CF-F54B-4045-9653-9E9B5A90ECEB}">
   <dimension ref="A8:A28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5746,132 +5761,133 @@
   <sheetData>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>ssxlibx2!A8&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M8,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M8, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M8,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M8, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M8, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M8, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M8, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M8, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M8, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M8, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M8, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M8,"0.00E+00")&amp;")"</f>
-        <v>TRISTATE BUFFER  =&gt;  ( ssxlib =&gt; 0.000E+00  , sxlib =&gt; 0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 021E+00 , 74act =&gt; 024E+00 , 74hc =&gt; 034E+00 , 74hct =&gt; 035E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A8 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M8,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M8,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M8,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M8, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M8, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M8, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M8, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M8, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M8, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M8, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M8, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M8,"0.00E+00")&amp;"),"</f>
+        <v>tristate_buffer =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 021E+00 , act =&gt; 024E+00 , hc =&gt; 034E+00 , hct =&gt; 035E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>ssxlibx2!A9&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M9,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M9, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M9,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M9, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M9, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M9, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M9, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M9, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M9, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M9, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M9, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M9,"0.00E+00")&amp;")"</f>
-        <v>BUFFER NON-INV  =&gt;  ( ssxlib =&gt; 017E+00  , sxlib =&gt; 017E+00 , vxlib =&gt; 018E+00 , vsclib =&gt; 013E+00 , wsclib =&gt; 013E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A9 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M9,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M9,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M9,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M9, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M9, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M9, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M9, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M9, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M9, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M9, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M9, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M9,"0.00E+00")&amp;"),"</f>
+        <v>buffer_non_inv =&gt;( ssxlib =&gt; 017E+00, sxlib =&gt;  017E+00 , vxlib =&gt; 018E+00 , vsclib =&gt; 013E+00 , wsclib =&gt; 013E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>ssxlibx2!A10&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M10,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M10, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M10,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M10, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M10, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M10, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M10, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M10, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M10, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M10, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M10, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M10,"0.00E+00")&amp;")"</f>
-        <v>INVERTER  =&gt;  ( ssxlib =&gt; 006E+00  , sxlib =&gt; 006E+00 , vxlib =&gt; 007E+00 , vsclib =&gt; 005E+00 , wsclib =&gt; 005E+00 , vgalib =&gt; 007E+00 , rgalib =&gt; 006E+00 , 74ac =&gt; 030E+00 , 74act =&gt; 030E+00 , 74hc =&gt; 021E+00 , 74hct =&gt; 024E+00 , cmos =&gt; 012E+00)</v>
+        <f>ssxlibx2!A10 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M10,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M10,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M10,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M10, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M10, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M10, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M10, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M10, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M10, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M10, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M10, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M10,"0.00E+00")&amp;"),"</f>
+        <v>inverter =&gt;( ssxlib =&gt; 006E+00, sxlib =&gt;  006E+00 , vxlib =&gt; 007E+00 , vsclib =&gt; 005E+00 , wsclib =&gt; 005E+00 , vgalib =&gt; 007E+00 , rgalib =&gt; 006E+00 , ac =&gt; 030E+00 , act =&gt; 030E+00 , hc =&gt; 021E+00 , hct =&gt; 024E+00 , cmos =&gt; 012E+00),</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>ssxlibx2!A11&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M11,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M11, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M11,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M11, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M11, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M11, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M11, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M11, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M11, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M11, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M11, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M11,"0.00E+00")&amp;")"</f>
-        <v>AND2  =&gt;  ( ssxlib =&gt; 020E+00  , sxlib =&gt; 020E+00 , vxlib =&gt; 020E+00 , vsclib =&gt; 015E+00 , wsclib =&gt; 015E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 020E+00 , 74act =&gt; 020E+00 , 74hc =&gt; 010E+00 , 74hct =&gt; 020E+00 , cmos =&gt; 018E+00)</v>
+        <f>ssxlibx2!A11 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M11,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M11,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M11,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M11, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M11, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M11, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M11, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M11, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M11, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M11, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M11, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M11,"0.00E+00")&amp;"),"</f>
+        <v>and2 =&gt;( ssxlib =&gt; 020E+00, sxlib =&gt;  020E+00 , vxlib =&gt; 020E+00 , vsclib =&gt; 015E+00 , wsclib =&gt; 015E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 020E+00 , act =&gt; 020E+00 , hc =&gt; 010E+00 , hct =&gt; 020E+00 , cmos =&gt; 018E+00),</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>ssxlibx2!A12&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M12,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M12, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M12,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M12, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M12, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M12, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M12, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M12, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M12, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M12, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M12, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M12,"0.00E+00")&amp;")"</f>
-        <v>AND3  =&gt;  ( ssxlib =&gt; 027E+00  , sxlib =&gt; 027E+00 , vxlib =&gt; 022E+00 , vsclib =&gt; 016E+00 , wsclib =&gt; 016E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A12 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M12,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M12,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M12,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M12, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M12, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M12, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M12, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M12, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M12, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M12, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M12, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M12,"0.00E+00")&amp;"),"</f>
+        <v>and3 =&gt;( ssxlib =&gt; 027E+00, sxlib =&gt;  027E+00 , vxlib =&gt; 022E+00 , vsclib =&gt; 016E+00 , wsclib =&gt; 016E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>ssxlibx2!A13&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M13,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M13, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M13,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M13, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M13, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M13, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M13, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M13, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M13, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M13, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M13, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M13,"0.00E+00")&amp;")"</f>
-        <v>AND4  =&gt;  ( ssxlib =&gt; 023E+00  , sxlib =&gt; 023E+00 , vxlib =&gt; 024E+00 , vsclib =&gt; 017E+00 , wsclib =&gt; 017E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A13 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M13,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M13,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M13,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M13, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M13, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M13, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M13, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M13, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M13, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M13, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M13, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M13,"0.00E+00")&amp;"),"</f>
+        <v>and4 =&gt;( ssxlib =&gt; 023E+00, sxlib =&gt;  023E+00 , vxlib =&gt; 024E+00 , vsclib =&gt; 017E+00 , wsclib =&gt; 017E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>ssxlibx2!A14&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M14,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M14, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M14,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M14, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M14, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M14, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M14, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M14, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M14, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M14, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M14, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M14,"0.00E+00")&amp;")"</f>
-        <v>OR2  =&gt;  ( ssxlib =&gt; 020E+00  , sxlib =&gt; 020E+00 , vxlib =&gt; 012E+00 , vsclib =&gt; 015E+00 , wsclib =&gt; 015E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 020E+00 , 74act =&gt; 020E+00 , 74hc =&gt; 016E+00 , 74hct =&gt; 028E+00 , cmos =&gt; 018E+00)</v>
+        <f>ssxlibx2!A14 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M14,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M14,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M14,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M14, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M14, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M14, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M14, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M14, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M14, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M14, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M14, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M14,"0.00E+00")&amp;"),"</f>
+        <v>or2 =&gt;( ssxlib =&gt; 020E+00, sxlib =&gt;  020E+00 , vxlib =&gt; 012E+00 , vsclib =&gt; 015E+00 , wsclib =&gt; 015E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 020E+00 , act =&gt; 020E+00 , hc =&gt; 016E+00 , hct =&gt; 028E+00 , cmos =&gt; 018E+00),</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>ssxlibx2!A15&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M15,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M15, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M15,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M15, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M15, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M15, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M15, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M15, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M15, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M15, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M15, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M15,"0.00E+00")&amp;")"</f>
-        <v>OR3  =&gt;  ( ssxlib =&gt; 021E+00  , sxlib =&gt; 021E+00 , vxlib =&gt; 014E+00 , vsclib =&gt; 016E+00 , wsclib =&gt; 016E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A15 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M15,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M15,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M15,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M15, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M15, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M15, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M15, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M15, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M15, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M15, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M15, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M15,"0.00E+00")&amp;"),"</f>
+        <v>or3 =&gt;( ssxlib =&gt; 021E+00, sxlib =&gt;  021E+00 , vxlib =&gt; 014E+00 , vsclib =&gt; 016E+00 , wsclib =&gt; 016E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>ssxlibx2!A16&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M16,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M16, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M16,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M16, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M16, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M16, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M16, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M16, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M16, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M16, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M16, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M16,"0.00E+00")&amp;")"</f>
-        <v>OR4  =&gt;  ( ssxlib =&gt; 022E+00  , sxlib =&gt; 022E+00 , vxlib =&gt; 014E+00 , vsclib =&gt; 017E+00 , wsclib =&gt; 017E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A16 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M16,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M16,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M16,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M16, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M16, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M16, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M16, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M16, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M16, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M16, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M16, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M16,"0.00E+00")&amp;"),"</f>
+        <v>or4 =&gt;( ssxlib =&gt; 022E+00, sxlib =&gt;  022E+00 , vxlib =&gt; 014E+00 , vsclib =&gt; 017E+00 , wsclib =&gt; 017E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>ssxlibx2!A17&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M17,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M17, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M17,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M17, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M17, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M17, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M17, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M17, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M17, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M17, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M17, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M17,"0.00E+00")&amp;")"</f>
-        <v>NAND2  =&gt;  ( ssxlib =&gt; 006E+00  , sxlib =&gt; 006E+00 , vxlib =&gt; 010E+00 , vsclib =&gt; 006E+00 , wsclib =&gt; 006E+00 , vgalib =&gt; 006E+00 , rgalib =&gt; 007E+00 , 74ac =&gt; 030E+00 , 74act =&gt; 030E+00 , 74hc =&gt; 022E+00 , 74hct =&gt; 022E+00 , cmos =&gt; 014E+00)</v>
+        <f>ssxlibx2!A17 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M17,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M17,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M17,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M17, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M17, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M17, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M17, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M17, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M17, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M17, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M17, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M17,"0.00E+00")&amp;"),"</f>
+        <v>nand2 =&gt;( ssxlib =&gt; 006E+00, sxlib =&gt;  006E+00 , vxlib =&gt; 010E+00 , vsclib =&gt; 006E+00 , wsclib =&gt; 006E+00 , vgalib =&gt; 006E+00 , rgalib =&gt; 007E+00 , ac =&gt; 030E+00 , act =&gt; 030E+00 , hc =&gt; 022E+00 , hct =&gt; 022E+00 , cmos =&gt; 014E+00),</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>ssxlibx2!A18&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M18,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M18, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M18,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M18, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M18, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M18, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M18, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M18, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M18, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M18, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M18, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M18,"0.00E+00")&amp;")"</f>
-        <v>NAND3  =&gt;  ( ssxlib =&gt; 008E+00  , sxlib =&gt; 008E+00 , vxlib =&gt; 012E+00 , vsclib =&gt; 009E+00 , wsclib =&gt; 009E+00 , vgalib =&gt; 009E+00 , rgalib =&gt; 010E+00 , 74ac =&gt; 025E+00 , 74act =&gt; 025E+00 , 74hc =&gt; 012E+00 , 74hct =&gt; 014E+00 , cmos =&gt; 017E+00)</v>
+        <f>ssxlibx2!A18 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M18,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M18,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M18,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M18, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M18, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M18, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M18, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M18, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M18, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M18, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M18, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M18,"0.00E+00")&amp;"),"</f>
+        <v>nand3 =&gt;( ssxlib =&gt; 008E+00, sxlib =&gt;  008E+00 , vxlib =&gt; 012E+00 , vsclib =&gt; 009E+00 , wsclib =&gt; 009E+00 , vgalib =&gt; 009E+00 , rgalib =&gt; 010E+00 , ac =&gt; 025E+00 , act =&gt; 025E+00 , hc =&gt; 012E+00 , hct =&gt; 014E+00 , cmos =&gt; 017E+00),</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>ssxlibx2!A19&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M19,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M19, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M19,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M19, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M19, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M19, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M19, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M19, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M19, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M19, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M19, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M19,"0.00E+00")&amp;")"</f>
-        <v>NAND4  =&gt;  ( ssxlib =&gt; 009E+00  , sxlib =&gt; 009E+00 , vxlib =&gt; 016E+00 , vsclib =&gt; 010E+00 , wsclib =&gt; 010E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 040E+00 , 74act =&gt; 033E+00 , 74hc =&gt; 022E+00 , 74hct =&gt; 017E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A19 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M19,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M19,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M19,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M19, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M19, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M19, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M19, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M19, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M19, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M19, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M19, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M19,"0.00E+00")&amp;"),"</f>
+        <v>nand4 =&gt;( ssxlib =&gt; 009E+00, sxlib =&gt;  009E+00 , vxlib =&gt; 016E+00 , vsclib =&gt; 010E+00 , wsclib =&gt; 010E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 040E+00 , act =&gt; 033E+00 , hc =&gt; 022E+00 , hct =&gt; 017E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>ssxlibx2!A20&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M20,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M20, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M20,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M20, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M20, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M20, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M20, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M20, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M20, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M20, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M20, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M20,"0.00E+00")&amp;")"</f>
-        <v>NOR2  =&gt;  ( ssxlib =&gt; 007E+00  , sxlib =&gt; 007E+00 , vxlib =&gt; 011E+00 , vsclib =&gt; 007E+00 , wsclib =&gt; 007E+00 , vgalib =&gt; 008E+00 , rgalib =&gt; 013E+00 , 74ac =&gt; 030E+00 , 74act =&gt; 030E+00 , 74hc =&gt; 022E+00 , 74hct =&gt; 024E+00 , cmos =&gt; 014E+00)</v>
+        <f>ssxlibx2!A20 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M20,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M20,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M20,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M20, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M20, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M20, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M20, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M20, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M20, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M20, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M20, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M20,"0.00E+00")&amp;"),"</f>
+        <v>nor2 =&gt;( ssxlib =&gt; 007E+00, sxlib =&gt;  007E+00 , vxlib =&gt; 011E+00 , vsclib =&gt; 007E+00 , wsclib =&gt; 007E+00 , vgalib =&gt; 008E+00 , rgalib =&gt; 013E+00 , ac =&gt; 030E+00 , act =&gt; 030E+00 , hc =&gt; 022E+00 , hct =&gt; 024E+00 , cmos =&gt; 014E+00),</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>ssxlibx2!A21&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M21,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M21, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M21,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M21, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M21, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M21, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M21, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M21, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M21, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M21, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M21, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M21,"0.00E+00")&amp;")"</f>
-        <v>NOR3  =&gt;  ( ssxlib =&gt; 008E+00  , sxlib =&gt; 008E+00 , vxlib =&gt; 012E+00 , vsclib =&gt; 012E+00 , wsclib =&gt; 012E+00 , vgalib =&gt; 010E+00 , rgalib =&gt; 016E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A21 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M21,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M21,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M21,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M21, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M21, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M21, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M21, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M21, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M21, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M21, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M21, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M21,"0.00E+00")&amp;"),"</f>
+        <v>nor3 =&gt;( ssxlib =&gt; 008E+00, sxlib =&gt;  008E+00 , vxlib =&gt; 012E+00 , vsclib =&gt; 012E+00 , wsclib =&gt; 012E+00 , vgalib =&gt; 010E+00 , rgalib =&gt; 016E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>ssxlibx2!A22&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M22,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M22, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M22,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M22, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M22, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M22, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M22, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M22, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M22, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M22, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M22, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M22,"0.00E+00")&amp;")"</f>
-        <v>NOR4  =&gt;  ( ssxlib =&gt; 008E+00  , sxlib =&gt; 008E+00 , vxlib =&gt; 035E+00 , vsclib =&gt; 012E+00 , wsclib =&gt; 012E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A22 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M22,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M22,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M22,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M22, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M22, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M22, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M22, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M22, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M22, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M22, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M22, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M22,"0.00E+00")&amp;"),"</f>
+        <v>nor4 =&gt;( ssxlib =&gt; 008E+00, sxlib =&gt;  008E+00 , vxlib =&gt; 035E+00 , vsclib =&gt; 012E+00 , wsclib =&gt; 012E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>ssxlibx2!A23&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M23,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M23, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M23,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M23, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M23, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M23, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M23, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M23, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M23, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M23, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M23, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M23,"0.00E+00")&amp;")"</f>
-        <v>XOR  =&gt;  ( ssxlib =&gt; 022E+00  , sxlib =&gt; 023E+00 , vxlib =&gt; 021E+00 , vsclib =&gt; 028E+00 , wsclib =&gt; 028E+00 , vgalib =&gt; 020E+00 , rgalib =&gt; 022E+00 , 74ac =&gt; 035E+00 , 74act =&gt; 030E+00 , 74hc =&gt; 030E+00 , 74hct =&gt; 030E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A23 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M23,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M23,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M23,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M23, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M23, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M23, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M23, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M23, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M23, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M23, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M23, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M23,"0.00E+00")&amp;"),"</f>
+        <v>xor2 =&gt;( ssxlib =&gt; 022E+00, sxlib =&gt;  023E+00 , vxlib =&gt; 021E+00 , vsclib =&gt; 028E+00 , wsclib =&gt; 028E+00 , vgalib =&gt; 020E+00 , rgalib =&gt; 022E+00 , ac =&gt; 035E+00 , act =&gt; 030E+00 , hc =&gt; 030E+00 , hct =&gt; 030E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>ssxlibx2!A24&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M24,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M24, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M24,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M24, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M24, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M24, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M24, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M24, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M24, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M24, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M24, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M24,"0.00E+00")&amp;")"</f>
-        <v>NXOR  =&gt;  ( ssxlib =&gt; 023E+00  , sxlib =&gt; 023E+00 , vxlib =&gt; 022E+00 , vsclib =&gt; 023E+00 , wsclib =&gt; 023E+00 , vgalib =&gt; 020E+00 , rgalib =&gt; 023E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 020E+00)</v>
+        <f>ssxlibx2!A24 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M24,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M24,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M24,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M24, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M24, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M24, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M24, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M24, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M24, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M24, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M24, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M24,"0.00E+00")&amp;"),"</f>
+        <v>xnor2 =&gt;( ssxlib =&gt; 023E+00, sxlib =&gt;  023E+00 , vxlib =&gt; 022E+00 , vsclib =&gt; 023E+00 , wsclib =&gt; 023E+00 , vgalib =&gt; 020E+00 , rgalib =&gt; 023E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 020E+00),</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>ssxlibx2!A25&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M25,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M25, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M25,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M25, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M25, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M25, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M25, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M25, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M25, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M25, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M25, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M25,"0.00E+00")&amp;")"</f>
-        <v>MUX2:1  =&gt;  ( ssxlib =&gt; 023E+00  , sxlib =&gt; 024E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 015E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A25 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M25,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M25,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M25,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M25, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M25, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M25, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M25, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M25, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M25, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M25, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M25, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M25,"0.00E+00")&amp;"),"</f>
+        <v>mux2 =&gt;( ssxlib =&gt; 023E+00, sxlib =&gt;  024E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 015E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>ssxlibx2!A26&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M26,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M26, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M26,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M26, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M26, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M26, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M26, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M26, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M26, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M26, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M26, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M26,"0.00E+00")&amp;")"</f>
-        <v>MUX4:1  =&gt;  ( ssxlib =&gt; 0.000E+00  , sxlib =&gt; 0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 040E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A26 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M26,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M26,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M26,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M26, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M26, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M26, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M26, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M26, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M26, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M26, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M26, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M26,"0.00E+00")&amp;"),"</f>
+        <v>mux4 =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 040E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>ssxlibx2!A27&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M27,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M27, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M27,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M27, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M27, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M27, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M27, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M27, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M27, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M27, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M27, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M27,"0.00E+00")&amp;")"</f>
-        <v>NUM163  =&gt;  ( ssxlib =&gt; 0.000E+00  , sxlib =&gt; 0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 060E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A27 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M27,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M27,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M27,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M27, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M27, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M27, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M27, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M27, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M27, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M27, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M27, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M27,"0.00E+00")&amp;"),"</f>
+        <v>num163 =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 060E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f>ssxlibx2!A28&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M28,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!M28, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M28,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M28, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M28, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M28, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M28, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!M28, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!M28, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!M28, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!M28, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M28,"0.00E+00")&amp;")"</f>
-        <v>DFF(rising edge)  =&gt;  ( ssxlib =&gt; 0.000E+00  , sxlib =&gt; 0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 009E+00 , wsclib =&gt; 009E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A28 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M28,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M28,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M28,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M28, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M28, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M28, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M28, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M28, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M28, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M28, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M28, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M28,"0.00E+00")&amp;"),"</f>
+        <v>dff_rising_edge =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 009E+00 , wsclib =&gt; 009E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5879,7 +5895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E03373BA-BC23-4613-8A11-3276A97CA114}">
   <dimension ref="A8:A28"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:A28"/>
     </sheetView>
   </sheetViews>
@@ -5890,132 +5906,133 @@
   <sheetData>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>ssxlibx2!A8&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N8,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N8, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N8,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N8, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N8, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N8, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N8, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N8, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N8, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N8, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N8, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N8,"0.00E+00")&amp;")"</f>
-        <v>TRISTATE BUFFER  =&gt;  ( ssxlib =&gt; 0.000E+00  , sxlib =&gt; 0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 004E+00 , 74act =&gt; 004E+00 , 74hc =&gt; 010E+00 , 74hct =&gt; 004E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A8 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N8,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N8,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N8,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N8, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N8, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N8, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N8, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N8, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N8, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N8, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N8, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N8,"0.00E+00")&amp;"),"</f>
+        <v>tristate_buffer =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 004E+00 , act =&gt; 004E+00 , hc =&gt; 010E+00 , hct =&gt; 004E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>ssxlibx2!A9&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N9,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N9, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N9,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N9, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N9, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N9, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N9, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N9, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N9, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N9, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N9, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N9,"0.00E+00")&amp;")"</f>
-        <v>BUFFER NON-INV  =&gt;  ( ssxlib =&gt; 003E+00  , sxlib =&gt; 003E+00 , vxlib =&gt; 005E+00 , vsclib =&gt; 003E+00 , wsclib =&gt; 003E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A9 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N9,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N9,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N9,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N9, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N9, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N9, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N9, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N9, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N9, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N9, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N9, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N9,"0.00E+00")&amp;"),"</f>
+        <v>buffer_non_inv =&gt;( ssxlib =&gt; 003E+00, sxlib =&gt;  003E+00 , vxlib =&gt; 005E+00 , vsclib =&gt; 003E+00 , wsclib =&gt; 003E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>ssxlibx2!A10&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N10,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N10, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N10,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N10, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N10, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N10, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N10, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N10, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N10, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N10, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N10, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N10,"0.00E+00")&amp;")"</f>
-        <v>INVERTER  =&gt;  ( ssxlib =&gt; 006E+00  , sxlib =&gt; 006E+00 , vxlib =&gt; 006E+00 , vsclib =&gt; 005E+00 , wsclib =&gt; 005E+00 , vgalib =&gt; 005E+00 , rgalib =&gt; 005E+00 , 74ac =&gt; 005E+00 , 74act =&gt; 005E+00 , 74hc =&gt; 004E+00 , 74hct =&gt; 004E+00 , cmos =&gt; 006E+00)</v>
+        <f>ssxlibx2!A10 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N10,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N10,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N10,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N10, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N10, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N10, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N10, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N10, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N10, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N10, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N10, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N10,"0.00E+00")&amp;"),"</f>
+        <v>inverter =&gt;( ssxlib =&gt; 006E+00, sxlib =&gt;  006E+00 , vxlib =&gt; 006E+00 , vsclib =&gt; 005E+00 , wsclib =&gt; 005E+00 , vgalib =&gt; 005E+00 , rgalib =&gt; 005E+00 , ac =&gt; 005E+00 , act =&gt; 005E+00 , hc =&gt; 004E+00 , hct =&gt; 004E+00 , cmos =&gt; 006E+00),</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>ssxlibx2!A11&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N11,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N11, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N11,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N11, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N11, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N11, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N11, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N11, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N11, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N11, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N11, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N11,"0.00E+00")&amp;")"</f>
-        <v>AND2  =&gt;  ( ssxlib =&gt; 005E+00  , sxlib =&gt; 005E+00 , vxlib =&gt; 006E+00 , vsclib =&gt; 004E+00 , wsclib =&gt; 004E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 005E+00 , 74act =&gt; 005E+00 , 74hc =&gt; 004E+00 , 74hct =&gt; 004E+00 , cmos =&gt; 005E+00)</v>
+        <f>ssxlibx2!A11 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N11,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N11,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N11,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N11, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N11, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N11, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N11, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N11, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N11, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N11, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N11, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N11,"0.00E+00")&amp;"),"</f>
+        <v>and2 =&gt;( ssxlib =&gt; 005E+00, sxlib =&gt;  005E+00 , vxlib =&gt; 006E+00 , vsclib =&gt; 004E+00 , wsclib =&gt; 004E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 005E+00 , act =&gt; 005E+00 , hc =&gt; 004E+00 , hct =&gt; 004E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>ssxlibx2!A12&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N12,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N12, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N12,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N12, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N12, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N12, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N12, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N12, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N12, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N12, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N12, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N12,"0.00E+00")&amp;")"</f>
-        <v>AND3  =&gt;  ( ssxlib =&gt; 005E+00  , sxlib =&gt; 005E+00 , vxlib =&gt; 006E+00 , vsclib =&gt; 004E+00 , wsclib =&gt; 004E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 005E+00)</v>
+        <f>ssxlibx2!A12 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N12,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N12,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N12,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N12, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N12, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N12, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N12, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N12, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N12, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N12, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N12, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N12,"0.00E+00")&amp;"),"</f>
+        <v>and3 =&gt;( ssxlib =&gt; 005E+00, sxlib =&gt;  005E+00 , vxlib =&gt; 006E+00 , vsclib =&gt; 004E+00 , wsclib =&gt; 004E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>ssxlibx2!A13&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N13,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N13, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N13,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N13, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N13, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N13, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N13, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N13, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N13, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N13, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N13, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N13,"0.00E+00")&amp;")"</f>
-        <v>AND4  =&gt;  ( ssxlib =&gt; 005E+00  , sxlib =&gt; 005E+00 , vxlib =&gt; 006E+00 , vsclib =&gt; 005E+00 , wsclib =&gt; 005E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A13 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N13,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N13,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N13,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N13, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N13, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N13, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N13, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N13, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N13, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N13, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N13, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N13,"0.00E+00")&amp;"),"</f>
+        <v>and4 =&gt;( ssxlib =&gt; 005E+00, sxlib =&gt;  005E+00 , vxlib =&gt; 006E+00 , vsclib =&gt; 005E+00 , wsclib =&gt; 005E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>ssxlibx2!A14&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N14,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N14, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N14,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N14, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N14, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N14, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N14, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N14, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N14, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N14, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N14, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N14,"0.00E+00")&amp;")"</f>
-        <v>OR2  =&gt;  ( ssxlib =&gt; 005E+00  , sxlib =&gt; 005E+00 , vxlib =&gt; 004E+00 , vsclib =&gt; 004E+00 , wsclib =&gt; 004E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 005E+00 , 74act =&gt; 005E+00 , 74hc =&gt; 004E+00 , 74hct =&gt; 004E+00 , cmos =&gt; 005E+00)</v>
+        <f>ssxlibx2!A14 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N14,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N14,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N14,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N14, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N14, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N14, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N14, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N14, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N14, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N14, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N14, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N14,"0.00E+00")&amp;"),"</f>
+        <v>or2 =&gt;( ssxlib =&gt; 005E+00, sxlib =&gt;  005E+00 , vxlib =&gt; 004E+00 , vsclib =&gt; 004E+00 , wsclib =&gt; 004E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 005E+00 , act =&gt; 005E+00 , hc =&gt; 004E+00 , hct =&gt; 004E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>ssxlibx2!A15&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N15,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N15, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N15,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N15, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N15, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N15, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N15, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N15, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N15, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N15, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N15, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N15,"0.00E+00")&amp;")"</f>
-        <v>OR3  =&gt;  ( ssxlib =&gt; 004E+00  , sxlib =&gt; 004E+00 , vxlib =&gt; 005E+00 , vsclib =&gt; 006E+00 , wsclib =&gt; 006E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 005E+00)</v>
+        <f>ssxlibx2!A15 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N15,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N15,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N15,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N15, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N15, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N15, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N15, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N15, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N15, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N15, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N15, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N15,"0.00E+00")&amp;"),"</f>
+        <v>or3 =&gt;( ssxlib =&gt; 004E+00, sxlib =&gt;  004E+00 , vxlib =&gt; 005E+00 , vsclib =&gt; 006E+00 , wsclib =&gt; 006E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>ssxlibx2!A16&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N16,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N16, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N16,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N16, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N16, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N16, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N16, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N16, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N16, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N16, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N16, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N16,"0.00E+00")&amp;")"</f>
-        <v>OR4  =&gt;  ( ssxlib =&gt; 004E+00  , sxlib =&gt; 004E+00 , vxlib =&gt; 005E+00 , vsclib =&gt; 006E+00 , wsclib =&gt; 006E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 008E+00)</v>
+        <f>ssxlibx2!A16 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N16,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N16,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N16,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N16, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N16, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N16, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N16, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N16, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N16, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N16, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N16, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N16,"0.00E+00")&amp;"),"</f>
+        <v>or4 =&gt;( ssxlib =&gt; 004E+00, sxlib =&gt;  004E+00 , vxlib =&gt; 005E+00 , vsclib =&gt; 006E+00 , wsclib =&gt; 006E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 008E+00),</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>ssxlibx2!A17&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N17,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N17, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N17,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N17, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N17, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N17, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N17, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N17, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N17, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N17, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N17, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N17,"0.00E+00")&amp;")"</f>
-        <v>NAND2  =&gt;  ( ssxlib =&gt; 004E+00  , sxlib =&gt; 004E+00 , vxlib =&gt; 008E+00 , vsclib =&gt; 005E+00 , wsclib =&gt; 005E+00 , vgalib =&gt; 005E+00 , rgalib =&gt; 005E+00 , 74ac =&gt; 005E+00 , 74act =&gt; 005E+00 , 74hc =&gt; 004E+00 , 74hct =&gt; 004E+00 , cmos =&gt; 005E+00)</v>
+        <f>ssxlibx2!A17 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N17,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N17,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N17,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N17, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N17, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N17, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N17, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N17, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N17, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N17, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N17, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N17,"0.00E+00")&amp;"),"</f>
+        <v>nand2 =&gt;( ssxlib =&gt; 004E+00, sxlib =&gt;  004E+00 , vxlib =&gt; 008E+00 , vsclib =&gt; 005E+00 , wsclib =&gt; 005E+00 , vgalib =&gt; 005E+00 , rgalib =&gt; 005E+00 , ac =&gt; 005E+00 , act =&gt; 005E+00 , hc =&gt; 004E+00 , hct =&gt; 004E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>ssxlibx2!A18&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N18,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N18, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N18,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N18, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N18, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N18, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N18, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N18, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N18, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N18, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N18, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N18,"0.00E+00")&amp;")"</f>
-        <v>NAND3  =&gt;  ( ssxlib =&gt; 005E+00  , sxlib =&gt; 005E+00 , vxlib =&gt; 007E+00 , vsclib =&gt; 006E+00 , wsclib =&gt; 006E+00 , vgalib =&gt; 005E+00 , rgalib =&gt; 005E+00 , 74ac =&gt; 005E+00 , 74act =&gt; 005E+00 , 74hc =&gt; 004E+00 , 74hct =&gt; 004E+00 , cmos =&gt; 005E+00)</v>
+        <f>ssxlibx2!A18 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N18,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N18,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N18,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N18, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N18, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N18, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N18, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N18, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N18, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N18, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N18, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N18,"0.00E+00")&amp;"),"</f>
+        <v>nand3 =&gt;( ssxlib =&gt; 005E+00, sxlib =&gt;  005E+00 , vxlib =&gt; 007E+00 , vsclib =&gt; 006E+00 , wsclib =&gt; 006E+00 , vgalib =&gt; 005E+00 , rgalib =&gt; 005E+00 , ac =&gt; 005E+00 , act =&gt; 005E+00 , hc =&gt; 004E+00 , hct =&gt; 004E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>ssxlibx2!A19&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N19,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N19, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N19,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N19, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N19, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N19, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N19, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N19, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N19, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N19, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N19, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N19,"0.00E+00")&amp;")"</f>
-        <v>NAND4  =&gt;  ( ssxlib =&gt; 004E+00  , sxlib =&gt; 005E+00 , vxlib =&gt; 009E+00 , vsclib =&gt; 006E+00 , wsclib =&gt; 006E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 005E+00 , 74act =&gt; 004E+00 , 74hc =&gt; 004E+00 , 74hct =&gt; 004E+00 , cmos =&gt; 005E+00)</v>
+        <f>ssxlibx2!A19 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N19,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N19,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N19,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N19, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N19, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N19, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N19, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N19, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N19, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N19, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N19, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N19,"0.00E+00")&amp;"),"</f>
+        <v>nand4 =&gt;( ssxlib =&gt; 004E+00, sxlib =&gt;  005E+00 , vxlib =&gt; 009E+00 , vsclib =&gt; 006E+00 , wsclib =&gt; 006E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 005E+00 , act =&gt; 004E+00 , hc =&gt; 004E+00 , hct =&gt; 004E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>ssxlibx2!A20&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N20,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N20, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N20,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N20, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N20, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N20, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N20, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N20, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N20, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N20, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N20, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N20,"0.00E+00")&amp;")"</f>
-        <v>NOR2  =&gt;  ( ssxlib =&gt; 005E+00  , sxlib =&gt; 005E+00 , vxlib =&gt; 010E+00 , vsclib =&gt; 007E+00 , wsclib =&gt; 007E+00 , vgalib =&gt; 007E+00 , rgalib =&gt; 010E+00 , 74ac =&gt; 005E+00 , 74act =&gt; 005E+00 , 74hc =&gt; 004E+00 , 74hct =&gt; 004E+00 , cmos =&gt; 005E+00)</v>
+        <f>ssxlibx2!A20 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N20,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N20,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N20,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N20, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N20, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N20, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N20, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N20, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N20, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N20, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N20, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N20,"0.00E+00")&amp;"),"</f>
+        <v>nor2 =&gt;( ssxlib =&gt; 005E+00, sxlib =&gt;  005E+00 , vxlib =&gt; 010E+00 , vsclib =&gt; 007E+00 , wsclib =&gt; 007E+00 , vgalib =&gt; 007E+00 , rgalib =&gt; 010E+00 , ac =&gt; 005E+00 , act =&gt; 005E+00 , hc =&gt; 004E+00 , hct =&gt; 004E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>ssxlibx2!A21&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N21,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N21, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N21,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N21, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N21, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N21, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N21, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N21, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N21, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N21, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N21, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N21,"0.00E+00")&amp;")"</f>
-        <v>NOR3  =&gt;  ( ssxlib =&gt; 005E+00  , sxlib =&gt; 005E+00 , vxlib =&gt; 009E+00 , vsclib =&gt; 010E+00 , wsclib =&gt; 010E+00 , vgalib =&gt; 007E+00 , rgalib =&gt; 010E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 005E+00)</v>
+        <f>ssxlibx2!A21 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N21,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N21,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N21,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N21, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N21, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N21, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N21, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N21, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N21, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N21, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N21, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N21,"0.00E+00")&amp;"),"</f>
+        <v>nor3 =&gt;( ssxlib =&gt; 005E+00, sxlib =&gt;  005E+00 , vxlib =&gt; 009E+00 , vsclib =&gt; 010E+00 , wsclib =&gt; 010E+00 , vgalib =&gt; 007E+00 , rgalib =&gt; 010E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>ssxlibx2!A22&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N22,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N22, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N22,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N22, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N22, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N22, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N22, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N22, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N22, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N22, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N22, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N22,"0.00E+00")&amp;")"</f>
-        <v>NOR4  =&gt;  ( ssxlib =&gt; 005E+00  , sxlib =&gt; 005E+00 , vxlib =&gt; 010E+00 , vsclib =&gt; 010E+00 , wsclib =&gt; 010E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 005E+00)</v>
+        <f>ssxlibx2!A22 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N22,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N22,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N22,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N22, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N22, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N22, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N22, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N22, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N22, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N22, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N22, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N22,"0.00E+00")&amp;"),"</f>
+        <v>nor4 =&gt;( ssxlib =&gt; 005E+00, sxlib =&gt;  005E+00 , vxlib =&gt; 010E+00 , vsclib =&gt; 010E+00 , wsclib =&gt; 010E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>ssxlibx2!A23&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N23,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N23, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N23,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N23, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N23, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N23, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N23, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N23, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N23, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N23, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N23, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N23,"0.00E+00")&amp;")"</f>
-        <v>XOR  =&gt;  ( ssxlib =&gt; 009E+00  , sxlib =&gt; 010E+00 , vxlib =&gt; 007E+00 , vsclib =&gt; 010E+00 , wsclib =&gt; 010E+00 , vgalib =&gt; 005E+00 , rgalib =&gt; 006E+00 , 74ac =&gt; 005E+00 , 74act =&gt; 005E+00 , 74hc =&gt; 004E+00 , 74hct =&gt; 004E+00 , cmos =&gt; 005E+00)</v>
+        <f>ssxlibx2!A23 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N23,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N23,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N23,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N23, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N23, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N23, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N23, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N23, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N23, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N23, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N23, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N23,"0.00E+00")&amp;"),"</f>
+        <v>xor2 =&gt;( ssxlib =&gt; 009E+00, sxlib =&gt;  010E+00 , vxlib =&gt; 007E+00 , vsclib =&gt; 010E+00 , wsclib =&gt; 010E+00 , vgalib =&gt; 005E+00 , rgalib =&gt; 006E+00 , ac =&gt; 005E+00 , act =&gt; 005E+00 , hc =&gt; 004E+00 , hct =&gt; 004E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>ssxlibx2!A24&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N24,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N24, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N24,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N24, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N24, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N24, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N24, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N24, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N24, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N24, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N24, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N24,"0.00E+00")&amp;")"</f>
-        <v>NXOR  =&gt;  ( ssxlib =&gt; 009E+00  , sxlib =&gt; 009E+00 , vxlib =&gt; 006E+00 , vsclib =&gt; 007E+00 , wsclib =&gt; 007E+00 , vgalib =&gt; 005E+00 , rgalib =&gt; 006E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 005E+00)</v>
+        <f>ssxlibx2!A24 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N24,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N24,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N24,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N24, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N24, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N24, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N24, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N24, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N24, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N24, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N24, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N24,"0.00E+00")&amp;"),"</f>
+        <v>xnor2 =&gt;( ssxlib =&gt; 009E+00, sxlib =&gt;  009E+00 , vxlib =&gt; 006E+00 , vsclib =&gt; 007E+00 , wsclib =&gt; 007E+00 , vgalib =&gt; 005E+00 , rgalib =&gt; 006E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>ssxlibx2!A25&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N25,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N25, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N25,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N25, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N25, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N25, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N25, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N25, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N25, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N25, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N25, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N25,"0.00E+00")&amp;")"</f>
-        <v>MUX2:1  =&gt;  ( ssxlib =&gt; 004E+00  , sxlib =&gt; 004E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 004E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A25 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N25,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N25,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N25,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N25, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N25, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N25, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N25, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N25, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N25, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N25, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N25, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N25,"0.00E+00")&amp;"),"</f>
+        <v>mux2 =&gt;( ssxlib =&gt; 004E+00, sxlib =&gt;  004E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 004E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>ssxlibx2!A26&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N26,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N26, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N26,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N26, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N26, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N26, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N26, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N26, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N26, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N26, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N26, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N26,"0.00E+00")&amp;")"</f>
-        <v>MUX4:1  =&gt;  ( ssxlib =&gt; 0.000E+00  , sxlib =&gt; 0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 004E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A26 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N26,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N26,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N26,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N26, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N26, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N26, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N26, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N26, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N26, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N26, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N26, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N26,"0.00E+00")&amp;"),"</f>
+        <v>mux4 =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 004E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>ssxlibx2!A27&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N27,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N27, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N27,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N27, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N27, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N27, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N27, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N27, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N27, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N27, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N27, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N27,"0.00E+00")&amp;")"</f>
-        <v>NUM163  =&gt;  ( ssxlib =&gt; 0.000E+00  , sxlib =&gt; 0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 004E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A27 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N27,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N27,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N27,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N27, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N27, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N27, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N27, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N27, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N27, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N27, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N27, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N27,"0.00E+00")&amp;"),"</f>
+        <v>num163 =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 004E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f>ssxlibx2!A28&amp;"  =&gt;  ( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N28,"0.00E+00") &amp; "  , sxlib =&gt; " &amp; TEXT(sxlibx2!N28, "0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N28,"0.00E+00") &amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N28, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N28, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N28, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N28, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!N28, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!N28, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!N28, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!N28, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N28,"0.00E+00")&amp;")"</f>
-        <v>DFF(rising edge)  =&gt;  ( ssxlib =&gt; 0.000E+00  , sxlib =&gt; 0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 002E+00 , wsclib =&gt; 002E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+        <f>ssxlibx2!A28 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N28,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N28,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N28,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N28, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N28, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N28, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N28, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N28, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N28, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N28, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N28, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N28,"0.00E+00")&amp;"),"</f>
+        <v>dff_rising_edge =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 002E+00 , wsclib =&gt; 002E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6023,8 +6040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3F6050-3A70-4B3E-887E-AAD3792C60E7}">
   <dimension ref="B8:B28"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6033,133 +6050,134 @@
   </cols>
   <sheetData>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="20" t="str">
-        <f>ssxlibx2!A8 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L8,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L8,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L8,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L8, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L8, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L8, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L8, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L8, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L8, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L8, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L8, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L8,"0.00E+00")&amp;")"</f>
-        <v>TRISTATE BUFFER =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 002E+00 , 74act =&gt; 008E+00 , 74hc =&gt; 004E+00 , 74hct =&gt; 008E+00 , cmos =&gt; 0.000E+00)</v>
+      <c r="B8" s="29" t="str">
+        <f>ssxlibx2!A8 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L8,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L8,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L8,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L8, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L8, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L8, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L8, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L8, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L8, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L8, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L8, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L8,"0.00E+00")&amp;"),"</f>
+        <v>tristate_buffer =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 002E+00 , act =&gt; 008E+00 , hc =&gt; 004E+00 , hct =&gt; 008E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="20" t="str">
-        <f>ssxlibx2!A9 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L9,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L9,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L9,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L9, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L9, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L9, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L9, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L9, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L9, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L9, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L9, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L9,"0.00E+00")&amp;")"</f>
-        <v>BUFFER NON-INV =&gt;( ssxlib =&gt; 7.333E-04, sxlib =&gt;  7.333E-04 , vxlib =&gt; 9.250E-04 , vsclib =&gt; 6.667E-04 , wsclib =&gt; 6.667E-04 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+      <c r="B9" s="29" t="str">
+        <f>ssxlibx2!A9 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L9,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L9,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L9,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L9, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L9, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L9, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L9, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L9, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L9, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L9, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L9, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L9,"0.00E+00")&amp;"),"</f>
+        <v>buffer_non_inv =&gt;( ssxlib =&gt; 7.333E-04, sxlib =&gt;  7.333E-04 , vxlib =&gt; 9.250E-04 , vsclib =&gt; 6.667E-04 , wsclib =&gt; 6.667E-04 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="str">
-        <f>ssxlibx2!A10 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L10,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L10,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L10,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L10, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L10, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L10, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L10, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L10, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L10, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L10, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L10, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L10,"0.00E+00")&amp;")"</f>
-        <v>INVERTER =&gt;( ssxlib =&gt; 4.833E-04, sxlib =&gt;  4.833E-04 , vxlib =&gt; 5.500E-04 , vsclib =&gt; 4.000E-04 , wsclib =&gt; 4.000E-04 , vgalib =&gt; 4.250E-04 , rgalib =&gt; 4.583E-04 , 74ac =&gt; 002E+00 , 74act =&gt; 004E+00 , 74hc =&gt; 002E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 010E+00)</v>
+      <c r="B10" s="29" t="str">
+        <f>ssxlibx2!A10 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L10,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L10,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L10,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L10, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L10, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L10, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L10, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L10, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L10, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L10, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L10, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L10,"0.00E+00")&amp;"),"</f>
+        <v>inverter =&gt;( ssxlib =&gt; 4.833E-04, sxlib =&gt;  4.833E-04 , vxlib =&gt; 5.500E-04 , vsclib =&gt; 4.000E-04 , wsclib =&gt; 4.000E-04 , vgalib =&gt; 4.250E-04 , rgalib =&gt; 4.583E-04 , ac =&gt; 002E+00 , act =&gt; 004E+00 , hc =&gt; 002E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 010E+00),</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="str">
-        <f>ssxlibx2!A11 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L11,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L11,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L11,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L11, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L11, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L11, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L11, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L11, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L11, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L11, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L11, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L11,"0.00E+00")&amp;")"</f>
-        <v>AND2 =&gt;( ssxlib =&gt; 9.667E-04, sxlib =&gt;  9.667E-04 , vxlib =&gt; 001E+00 , vsclib =&gt; 8.917E-04 , wsclib =&gt; 8.917E-04 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 002E+00 , 74act =&gt; 004E+00 , 74hc =&gt; 002E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 004E+00)</v>
+      <c r="B11" s="29" t="str">
+        <f>ssxlibx2!A11 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L11,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L11,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L11,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L11, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L11, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L11, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L11, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L11, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L11, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L11, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L11, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L11,"0.00E+00")&amp;"),"</f>
+        <v>and2 =&gt;( ssxlib =&gt; 9.667E-04, sxlib =&gt;  9.667E-04 , vxlib =&gt; 001E+00 , vsclib =&gt; 8.917E-04 , wsclib =&gt; 8.917E-04 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 002E+00 , act =&gt; 004E+00 , hc =&gt; 002E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 004E+00),</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="str">
-        <f>ssxlibx2!A12 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L12,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L12,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L12,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L12, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L12, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L12, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L12, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L12, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L12, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L12, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L12, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L12,"0.00E+00")&amp;")"</f>
-        <v>AND3 =&gt;( ssxlib =&gt; 001E+00, sxlib =&gt;  001E+00 , vxlib =&gt; 001E+00 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 010E+00)</v>
+      <c r="B12" s="29" t="str">
+        <f>ssxlibx2!A12 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L12,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L12,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L12,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L12, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L12, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L12, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L12, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L12, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L12, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L12, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L12, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L12,"0.00E+00")&amp;"),"</f>
+        <v>and3 =&gt;( ssxlib =&gt; 001E+00, sxlib =&gt;  001E+00 , vxlib =&gt; 001E+00 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 010E+00),</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="str">
-        <f>ssxlibx2!A13 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L13,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L13,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L13,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L13, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L13, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L13, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L13, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L13, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L13, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L13, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L13, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L13,"0.00E+00")&amp;")"</f>
-        <v>AND4 =&gt;( ssxlib =&gt; 002E+00, sxlib =&gt;  002E+00 , vxlib =&gt; 002E+00 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 010E+00)</v>
+      <c r="B13" s="29" t="str">
+        <f>ssxlibx2!A13 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L13,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L13,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L13,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L13, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L13, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L13, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L13, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L13, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L13, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L13, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L13, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L13,"0.00E+00")&amp;"),"</f>
+        <v>and4 =&gt;( ssxlib =&gt; 002E+00, sxlib =&gt;  002E+00 , vxlib =&gt; 002E+00 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 010E+00),</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="20" t="str">
-        <f>ssxlibx2!A14 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L14,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L14,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L14,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L14, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L14, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L14, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L14, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L14, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L14, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L14, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L14, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L14,"0.00E+00")&amp;")"</f>
-        <v>OR2 =&gt;( ssxlib =&gt; 001E+00, sxlib =&gt;  001E+00 , vxlib =&gt; 6.833E-04 , vsclib =&gt; 8.250E-04 , wsclib =&gt; 8.250E-04 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 002E+00 , 74act =&gt; 004E+00 , 74hc =&gt; 002E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 004E+00)</v>
+      <c r="B14" s="29" t="str">
+        <f>ssxlibx2!A14 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L14,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L14,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L14,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L14, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L14, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L14, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L14, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L14, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L14, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L14, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L14, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L14,"0.00E+00")&amp;"),"</f>
+        <v>or2 =&gt;( ssxlib =&gt; 001E+00, sxlib =&gt;  001E+00 , vxlib =&gt; 6.833E-04 , vsclib =&gt; 8.250E-04 , wsclib =&gt; 8.250E-04 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 002E+00 , act =&gt; 004E+00 , hc =&gt; 002E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 004E+00),</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="str">
-        <f>ssxlibx2!A15 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L15,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L15,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L15,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L15, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L15, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L15, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L15, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L15, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L15, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L15, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L15, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L15,"0.00E+00")&amp;")"</f>
-        <v>OR3 =&gt;( ssxlib =&gt; 001E+00, sxlib =&gt;  001E+00 , vxlib =&gt; 8.500E-04 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 010E+00)</v>
+      <c r="B15" s="29" t="str">
+        <f>ssxlibx2!A15 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L15,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L15,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L15,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L15, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L15, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L15, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L15, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L15, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L15, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L15, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L15, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L15,"0.00E+00")&amp;"),"</f>
+        <v>or3 =&gt;( ssxlib =&gt; 001E+00, sxlib =&gt;  001E+00 , vxlib =&gt; 8.500E-04 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 010E+00),</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="str">
-        <f>ssxlibx2!A16 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L16,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L16,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L16,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L16, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L16, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L16, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L16, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L16, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L16, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L16, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L16, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L16,"0.00E+00")&amp;")"</f>
-        <v>OR4 =&gt;( ssxlib =&gt; 001E+00, sxlib =&gt;  001E+00 , vxlib =&gt; 8.917E-04 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 250E+00)</v>
+      <c r="B16" s="29" t="str">
+        <f>ssxlibx2!A16 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L16,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L16,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L16,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L16, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L16, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L16, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L16, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L16, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L16, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L16, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L16, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L16,"0.00E+00")&amp;"),"</f>
+        <v>or4 =&gt;( ssxlib =&gt; 001E+00, sxlib =&gt;  001E+00 , vxlib =&gt; 8.917E-04 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 250E+00),</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="str">
-        <f>ssxlibx2!A17 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L17,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L17,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L17,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L17, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L17, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L17, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L17, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L17, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L17, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L17, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L17, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L17,"0.00E+00")&amp;")"</f>
-        <v>NAND2 =&gt;( ssxlib =&gt; 5.750E-04, sxlib =&gt;  5.750E-04 , vxlib =&gt; 001E+00 , vsclib =&gt; 6.583E-04 , wsclib =&gt; 6.583E-04 , vgalib =&gt; 6.750E-04 , rgalib =&gt; 7.333E-04 , 74ac =&gt; 002E+00 , 74act =&gt; 002E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 004E+00)</v>
+      <c r="B17" s="29" t="str">
+        <f>ssxlibx2!A17 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L17,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L17,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L17,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L17, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L17, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L17, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L17, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L17, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L17, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L17, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L17, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L17,"0.00E+00")&amp;"),"</f>
+        <v>nand2 =&gt;( ssxlib =&gt; 5.750E-04, sxlib =&gt;  5.750E-04 , vxlib =&gt; 001E+00 , vsclib =&gt; 6.583E-04 , wsclib =&gt; 6.583E-04 , vgalib =&gt; 6.750E-04 , rgalib =&gt; 7.333E-04 , ac =&gt; 002E+00 , act =&gt; 002E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 004E+00),</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="str">
-        <f>ssxlibx2!A18 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L18,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L18,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L18,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L18, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L18, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L18, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L18, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L18, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L18, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L18, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L18, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L18,"0.00E+00")&amp;")"</f>
-        <v>NAND3 =&gt;( ssxlib =&gt; 7.667E-04, sxlib =&gt;  7.667E-04 , vxlib =&gt; 001E+00 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 9.250E-04 , rgalib =&gt; 001E+00 , 74ac =&gt; 002E+00 , 74act =&gt; 004E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 004E+00)</v>
+      <c r="B18" s="29" t="str">
+        <f>ssxlibx2!A18 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L18,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L18,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L18,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L18, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L18, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L18, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L18, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L18, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L18, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L18, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L18, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L18,"0.00E+00")&amp;"),"</f>
+        <v>nand3 =&gt;( ssxlib =&gt; 7.667E-04, sxlib =&gt;  7.667E-04 , vxlib =&gt; 001E+00 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 9.250E-04 , rgalib =&gt; 001E+00 , ac =&gt; 002E+00 , act =&gt; 004E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 004E+00),</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="str">
-        <f>ssxlibx2!A19 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L19,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L19,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L19,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L19, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L19, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L19, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L19, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L19, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L19, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L19, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L19, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L19,"0.00E+00")&amp;")"</f>
-        <v>NAND4 =&gt;( ssxlib =&gt; 9.667E-04, sxlib =&gt;  9.667E-04 , vxlib =&gt; 002E+00 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 002E+00 , 74act =&gt; 004E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 005E+00)</v>
+      <c r="B19" s="29" t="str">
+        <f>ssxlibx2!A19 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L19,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L19,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L19,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L19, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L19, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L19, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L19, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L19, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L19, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L19, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L19, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L19,"0.00E+00")&amp;"),"</f>
+        <v>nand4 =&gt;( ssxlib =&gt; 9.667E-04, sxlib =&gt;  9.667E-04 , vxlib =&gt; 002E+00 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 002E+00 , act =&gt; 004E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="str">
-        <f>ssxlibx2!A20 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L20,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L20,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L20,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L20, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L20, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L20, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L20, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L20, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L20, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L20, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L20, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L20,"0.00E+00")&amp;")"</f>
-        <v>NOR2 =&gt;( ssxlib =&gt; 5.750E-04, sxlib =&gt;  5.750E-04 , vxlib =&gt; 001E+00 , vsclib =&gt; 8.083E-04 , wsclib =&gt; 8.083E-04 , vgalib =&gt; 6.750E-04 , rgalib =&gt; 001E+00 , 74ac =&gt; 002E+00 , 74act =&gt; 004E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 004E+00)</v>
+      <c r="B20" s="29" t="str">
+        <f>ssxlibx2!A20 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L20,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L20,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L20,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L20, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L20, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L20, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L20, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L20, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L20, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L20, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L20, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L20,"0.00E+00")&amp;"),"</f>
+        <v>nor2 =&gt;( ssxlib =&gt; 5.750E-04, sxlib =&gt;  5.750E-04 , vxlib =&gt; 001E+00 , vsclib =&gt; 8.083E-04 , wsclib =&gt; 8.083E-04 , vgalib =&gt; 6.750E-04 , rgalib =&gt; 001E+00 , ac =&gt; 002E+00 , act =&gt; 004E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 004E+00),</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="str">
-        <f>ssxlibx2!A21 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L21,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L21,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L21,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L21, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L21, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L21, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L21, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L21, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L21, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L21, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L21, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L21,"0.00E+00")&amp;")"</f>
-        <v>NOR3 =&gt;( ssxlib =&gt; 6.750E-04, sxlib =&gt;  6.750E-04 , vxlib =&gt; 001E+00 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 002E+00 , rgalib =&gt; 002E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 005E+00)</v>
+      <c r="B21" s="29" t="str">
+        <f>ssxlibx2!A21 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L21,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L21,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L21,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L21, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L21, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L21, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L21, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L21, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L21, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L21, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L21, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L21,"0.00E+00")&amp;"),"</f>
+        <v>nor3 =&gt;( ssxlib =&gt; 6.750E-04, sxlib =&gt;  6.750E-04 , vxlib =&gt; 001E+00 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 002E+00 , rgalib =&gt; 002E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="str">
-        <f>ssxlibx2!A22 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L22,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L22,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L22,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L22, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L22, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L22, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L22, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L22, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L22, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L22, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L22, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L22,"0.00E+00")&amp;")"</f>
-        <v>NOR4 =&gt;( ssxlib =&gt; 7.667E-04, sxlib =&gt;  7.667E-04 , vxlib =&gt; 001E+00 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 005E+00)</v>
+      <c r="B22" s="29" t="str">
+        <f>ssxlibx2!A22 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L22,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L22,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L22,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L22, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L22, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L22, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L22, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L22, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L22, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L22, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L22, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L22,"0.00E+00")&amp;"),"</f>
+        <v>nor4 =&gt;( ssxlib =&gt; 7.667E-04, sxlib =&gt;  7.667E-04 , vxlib =&gt; 001E+00 , vsclib =&gt; 001E+00 , wsclib =&gt; 001E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 005E+00),</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="20" t="str">
-        <f>ssxlibx2!A23 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L23,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L23,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L23,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L23, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L23, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L23, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L23, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L23, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L23, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L23, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L23, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L23,"0.00E+00")&amp;")"</f>
-        <v>XOR =&gt;( ssxlib =&gt; 002E+00, sxlib =&gt;  002E+00 , vxlib =&gt; 001E+00 , vsclib =&gt; 002E+00 , wsclib =&gt; 002E+00 , vgalib =&gt; 001E+00 , rgalib =&gt; 001E+00 , 74ac =&gt; 002E+00 , 74act =&gt; 002E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 050E+00)</v>
+      <c r="B23" s="29" t="str">
+        <f>ssxlibx2!A23 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L23,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L23,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L23,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L23, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L23, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L23, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L23, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L23, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L23, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L23, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L23, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L23,"0.00E+00")&amp;"),"</f>
+        <v>xor2 =&gt;( ssxlib =&gt; 002E+00, sxlib =&gt;  002E+00 , vxlib =&gt; 001E+00 , vsclib =&gt; 002E+00 , wsclib =&gt; 002E+00 , vgalib =&gt; 001E+00 , rgalib =&gt; 001E+00 , ac =&gt; 002E+00 , act =&gt; 002E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 050E+00),</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="str">
-        <f>ssxlibx2!A24 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L24,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L24,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L24,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L24, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L24, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L24, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L24, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L24, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L24, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L24, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L24, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L24,"0.00E+00")&amp;")"</f>
-        <v>NXOR =&gt;( ssxlib =&gt; 002E+00, sxlib =&gt;  002E+00 , vxlib =&gt; 001E+00 , vsclib =&gt; 002E+00 , wsclib =&gt; 002E+00 , vgalib =&gt; 001E+00 , rgalib =&gt; 001E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 100E+00)</v>
+      <c r="B24" s="29" t="str">
+        <f>ssxlibx2!A24 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L24,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L24,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L24,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L24, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L24, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L24, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L24, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L24, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L24, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L24, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L24, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L24,"0.00E+00")&amp;"),"</f>
+        <v>xnor2 =&gt;( ssxlib =&gt; 002E+00, sxlib =&gt;  002E+00 , vxlib =&gt; 001E+00 , vsclib =&gt; 002E+00 , wsclib =&gt; 002E+00 , vgalib =&gt; 001E+00 , rgalib =&gt; 001E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 100E+00),</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="20" t="str">
-        <f>ssxlibx2!A25 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L25,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L25,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L25,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L25, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L25, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L25, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L25, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L25, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L25, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L25, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L25, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L25,"0.00E+00")&amp;")"</f>
-        <v>MUX2:1 =&gt;( ssxlib =&gt; 001E+00, sxlib =&gt;  001E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 8.583E-04 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+      <c r="B25" s="29" t="str">
+        <f>ssxlibx2!A25 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L25,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L25,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L25,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L25, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L25, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L25, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L25, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L25, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L25, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L25, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L25, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L25,"0.00E+00")&amp;"),"</f>
+        <v>mux2 =&gt;( ssxlib =&gt; 001E+00, sxlib =&gt;  001E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 8.583E-04 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="20" t="str">
-        <f>ssxlibx2!A26 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L26,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L26,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L26,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L26, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L26, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L26, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L26, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L26, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L26, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L26, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L26, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L26,"0.00E+00")&amp;")"</f>
-        <v>MUX4:1 =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 008E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+      <c r="B26" s="29" t="str">
+        <f>ssxlibx2!A26 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L26,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L26,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L26,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L26, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L26, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L26, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L26, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L26, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L26, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L26, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L26, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L26,"0.00E+00")&amp;"),"</f>
+        <v>mux4 =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 008E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="20" t="str">
-        <f>ssxlibx2!A27 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L27,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L27,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L27,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L27, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L27, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L27, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L27, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L27, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L27, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L27, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L27, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L27,"0.00E+00")&amp;")"</f>
-        <v>NUM163 =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 008E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+      <c r="B27" s="29" t="str">
+        <f>ssxlibx2!A27 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L27,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L27,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L27,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L27, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L27, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L27, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L27, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L27, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L27, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L27, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L27, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L27,"0.00E+00")&amp;"),"</f>
+        <v>num163 =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 008E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="20" t="str">
-        <f>ssxlibx2!A28 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L28,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L28,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L28,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L28, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L28, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L28, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L28, "0.00E+00") &amp; " , 74ac =&gt; " &amp; TEXT('74ac'!L28, "0.00E+00") &amp; " , 74act =&gt; " &amp; TEXT('74act'!L28, "0.00E+00") &amp; " , 74hc =&gt; " &amp; TEXT('74hc'!L28, "0.00E+00") &amp; " , 74hct =&gt; " &amp; TEXT('74hct'!L28, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L28,"0.00E+00")&amp;")"</f>
-        <v>DFF(rising edge) =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 002E+00 , wsclib =&gt; 002E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , 74ac =&gt; 0.000E+00 , 74act =&gt; 0.000E+00 , 74hc =&gt; 0.000E+00 , 74hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00)</v>
+      <c r="B28" s="29" t="str">
+        <f>ssxlibx2!A28 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L28,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L28,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L28,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L28, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L28, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L28, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L28, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L28, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L28, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L28, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L28, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L28,"0.00E+00")&amp;"),"</f>
+        <v>dff_rising_edge =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 002E+00 , wsclib =&gt; 002E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6168,7 +6186,7 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="L8" sqref="L8:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6187,16 +6205,16 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6204,13 +6222,13 @@
         <v>1.2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -6219,49 +6237,49 @@
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="27" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="24" t="s">
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="23"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="22"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
@@ -6283,7 +6301,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>13</v>
@@ -6298,27 +6316,27 @@
         <v>12</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B8" s="14">
         <v>0</v>
@@ -6377,7 +6395,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>1.3</v>
@@ -6436,7 +6454,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -6495,7 +6513,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3">
         <v>1.7</v>
@@ -6554,7 +6572,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -6613,7 +6631,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>2.2999999999999998</v>
@@ -6672,7 +6690,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B14">
         <v>1.7</v>
@@ -6731,7 +6749,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -6790,7 +6808,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B16">
         <v>2.2999999999999998</v>
@@ -6849,7 +6867,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>1.3</v>
@@ -6908,7 +6926,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="B18">
         <v>1.7</v>
@@ -6967,7 +6985,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -7026,7 +7044,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B20">
         <v>1.3</v>
@@ -7085,7 +7103,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="B21">
         <v>1.7</v>
@@ -7144,7 +7162,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -7203,7 +7221,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -7262,7 +7280,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -7321,7 +7339,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -7380,7 +7398,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -7439,7 +7457,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -7498,7 +7516,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -7577,8 +7595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40EC2ACA-1533-4922-94A4-1C2062C36F9B}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7593,16 +7611,16 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7610,13 +7628,13 @@
         <v>1.2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -7625,49 +7643,49 @@
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="27" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="24" t="s">
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="23"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="22"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
@@ -7689,7 +7707,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>13</v>
@@ -7704,27 +7722,27 @@
         <v>12</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B8" s="14">
         <v>0</v>
@@ -7783,7 +7801,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>1.3</v>
@@ -7842,7 +7860,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -7901,7 +7919,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3">
         <v>1.7</v>
@@ -7960,7 +7978,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -8019,7 +8037,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>2.2999999999999998</v>
@@ -8078,7 +8096,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B14">
         <v>1.7</v>
@@ -8137,7 +8155,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -8196,7 +8214,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B16">
         <v>2.2999999999999998</v>
@@ -8255,7 +8273,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>1.3</v>
@@ -8314,7 +8332,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B18">
         <v>1.7</v>
@@ -8373,7 +8391,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -8432,7 +8450,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B20">
         <v>1.3</v>
@@ -8491,7 +8509,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="B21">
         <v>1.7</v>
@@ -8550,7 +8568,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -8609,7 +8627,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -8668,7 +8686,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -8727,7 +8745,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -8786,7 +8804,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -8845,7 +8863,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -8904,7 +8922,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -8979,8 +8997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8931ED3F-218D-49ED-B1A9-4698AB234161}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:K28"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8993,16 +9011,16 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9010,13 +9028,13 @@
         <v>1.2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -9025,49 +9043,49 @@
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="27" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="24" t="s">
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="23"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="22"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
@@ -9089,7 +9107,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>13</v>
@@ -9104,27 +9122,27 @@
         <v>12</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B8" s="14">
         <v>0</v>
@@ -9183,7 +9201,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>1.3</v>
@@ -9242,7 +9260,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -9301,7 +9319,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3">
         <v>1.7</v>
@@ -9360,7 +9378,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -9419,7 +9437,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>2.2999999999999998</v>
@@ -9478,7 +9496,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B14">
         <v>1.7</v>
@@ -9537,7 +9555,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -9596,7 +9614,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B16">
         <v>2.7</v>
@@ -9655,7 +9673,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>1.3</v>
@@ -9714,7 +9732,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B18">
         <v>1.7</v>
@@ -9773,7 +9791,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -9832,7 +9850,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -9891,7 +9909,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="B21">
         <v>2.2999999999999998</v>
@@ -9950,7 +9968,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -10009,7 +10027,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B23">
         <v>2.2999999999999998</v>
@@ -10068,7 +10086,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B24">
         <v>2.2999999999999998</v>
@@ -10127,7 +10145,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -10186,7 +10204,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -10245,7 +10263,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -10304,7 +10322,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -10379,8 +10397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B16F2BC-9B4C-4AD0-9117-267F85A79AE3}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:K27"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10394,16 +10412,16 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10411,13 +10429,13 @@
         <v>1.2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -10426,49 +10444,49 @@
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="27" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="24" t="s">
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="23"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="22"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
@@ -10490,7 +10508,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>13</v>
@@ -10505,27 +10523,27 @@
         <v>12</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B8" s="14">
         <v>0</v>
@@ -10584,7 +10602,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>1.3</v>
@@ -10643,7 +10661,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -10702,7 +10720,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3">
         <v>1.7</v>
@@ -10761,7 +10779,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>2.2999999999999998</v>
@@ -10820,7 +10838,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>2.7</v>
@@ -10879,7 +10897,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B14">
         <v>1.7</v>
@@ -10938,7 +10956,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -10997,7 +11015,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B16">
         <v>3.7</v>
@@ -11056,7 +11074,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>1.3</v>
@@ -11115,7 +11133,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B18">
         <v>2.7</v>
@@ -11174,7 +11192,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="B19">
         <v>3.3</v>
@@ -11233,7 +11251,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -11292,7 +11310,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="B21">
         <v>3.7</v>
@@ -11351,7 +11369,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B22">
         <v>4.7</v>
@@ -11410,7 +11428,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B23">
         <v>4.7</v>
@@ -11469,7 +11487,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B24">
         <v>4.3</v>
@@ -11528,7 +11546,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -11587,7 +11605,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -11646,7 +11664,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -11705,7 +11723,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B28">
         <v>6</v>
@@ -11780,8 +11798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3909F10-6235-4E59-ABD1-9231BF023B6B}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11795,16 +11813,16 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11812,13 +11830,13 @@
         <v>1.2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -11827,49 +11845,49 @@
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="27" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="24" t="s">
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="K6" s="26"/>
-      <c r="L6" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="23"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="21"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="22"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
@@ -11891,7 +11909,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>13</v>
@@ -11906,27 +11924,27 @@
         <v>12</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="Q7" s="9" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B8" s="14">
         <v>0</v>
@@ -11985,7 +12003,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>1.3</v>
@@ -12044,7 +12062,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -12103,7 +12121,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3">
         <v>1.7</v>
@@ -12162,7 +12180,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B12">
         <v>2.2999999999999998</v>
@@ -12221,7 +12239,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="B13">
         <v>2.7</v>
@@ -12280,7 +12298,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B14">
         <v>1.7</v>
@@ -12339,7 +12357,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -12398,7 +12416,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B16">
         <v>3.7</v>
@@ -12457,7 +12475,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B17">
         <v>1.3</v>
@@ -12516,7 +12534,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B18">
         <v>2.7</v>
@@ -12575,7 +12593,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="B19">
         <v>3.3</v>
@@ -12634,7 +12652,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -12693,7 +12711,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="B21">
         <v>3.7</v>
@@ -12752,7 +12770,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B22">
         <v>4.7</v>
@@ -12811,7 +12829,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B23">
         <v>4.7</v>
@@ -12870,7 +12888,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B24">
         <v>4.3</v>
@@ -12929,7 +12947,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="B25">
         <v>2.7</v>
@@ -12988,7 +13006,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -13047,7 +13065,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -13106,7 +13124,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B28">
         <v>6</v>

</xml_diff>

<commit_message>
final updates Signed-off-by: Iulia Chereja <chereja_iulia@yahoo.com>
</commit_message>
<xml_diff>
--- a/src/PELib/gates.xlsx
+++ b/src/PELib/gates.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C01257F6-1A62-4C18-AF6F-5528995CE74B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055D6724-4EE2-4B15-9A92-41D1A1BB8C8C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8130" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -716,7 +716,7 @@
   <dimension ref="A2:C28"/>
   <sheetViews>
     <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C28"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,8 +743,8 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="str">
-        <f>ssxlibx2!A8 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q8*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q8*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q8*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q8*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q8*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q8*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q8*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q8*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q8*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q8*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q8*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q8*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>tristate_buffer =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <f>ssxlibx2!A8 &amp; " =&gt;( C7ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q8*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q8*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q8*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q8*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q8*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q8*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q8*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q8*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q8*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q8*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q8*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q8*mm*mm,"0.00E+00")&amp;"),"</f>
+        <v>tristate_buffer =&gt;( C7ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -4100,8 +4100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3D0F2B-832D-4300-97D5-DDEB6D07CF40}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5369,7 +5369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DCB8990-16FC-4DA4-A64E-185EE2DC6D83}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:A28"/>
     </sheetView>
   </sheetViews>
@@ -5954,7 +5954,7 @@
   <dimension ref="B2:C28"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C28"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5971,7 +5971,7 @@
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C8" t="str">
         <f>ssxlibx2!A8 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N8*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N8*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N8*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N8*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N8*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N8*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N8*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N8*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N8*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N8*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N8*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N8*pF,"0.00E+00")&amp;"),"</f>
-        <v>tristate_buffer =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 4.00E-12 , act =&gt; 4.00E-12 , hc =&gt; 1.00E-11 , hct =&gt; 3.50E-12 , cmos =&gt; 0.00E+00),</v>
+        <v>tristate_buffer =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 004E-12 , act =&gt; 004E-12 , hc =&gt; 010E-12 , hct =&gt; 004E-12 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -6105,7 +6105,7 @@
   <dimension ref="A2:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6131,128 +6131,128 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" s="20" t="str">
-        <f>ssxlibx2!A8 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L8*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L8*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L8*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L8*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L8*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L8*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L8*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L8*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L8*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L8*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L8*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L8*uA,"0.00E+00")&amp;"),"</f>
-        <v>tristate_buffer =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 2.00E-06 , act =&gt; 8.00E-06 , hc =&gt; 4.00E-06 , hct =&gt; 8.00E-06 , cmos =&gt; 0.00E+00),</v>
+        <f>ssxlibx2!A8 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L8*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L8*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L8*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L8*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L8*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L8*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L8*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L8*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L8*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L8*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L8*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L8*nA,"0.00E+00")&amp;"),"</f>
+        <v>tristate_buffer =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 200E-08 , act =&gt; 800E-08 , hc =&gt; 400E-08 , hct =&gt; 800E-08 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" s="20" t="str">
-        <f>ssxlibx2!A9 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L9*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L9*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L9*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L9*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L9*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L9*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L9*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L9*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L9*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L9*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L9*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L9*uA,"0.00E+00")&amp;"),"</f>
-        <v>buffer_non_inv =&gt;( ssxlib =&gt; 7.33E-10, sxlib =&gt;  7.33E-10 , vxlib =&gt; 9.25E-10 , vsclib =&gt; 6.67E-10 , wsclib =&gt; 6.67E-10 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <f>ssxlibx2!A9 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L9*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L9*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L9*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L9*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L9*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L9*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L9*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L9*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L9*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L9*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L9*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L9*nA,"0.00E+00")&amp;"),"</f>
+        <v>buffer_non_inv =&gt;( ssxlib =&gt; 733E-12, sxlib =&gt;  733E-12 , vxlib =&gt; 925E-12 , vsclib =&gt; 667E-12 , wsclib =&gt; 667E-12 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C10" s="20" t="str">
-        <f>ssxlibx2!A10 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L10*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L10*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L10*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L10*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L10*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L10*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L10*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L10*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L10*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L10*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L10*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L10*uA,"0.00E+00")&amp;"),"</f>
-        <v>inverter =&gt;( ssxlib =&gt; 4.83E-10, sxlib =&gt;  4.83E-10 , vxlib =&gt; 5.50E-10 , vsclib =&gt; 4.00E-10 , wsclib =&gt; 4.00E-10 , vgalib =&gt; 4.25E-10 , rgalib =&gt; 4.58E-10 , ac =&gt; 2.00E-06 , act =&gt; 4.00E-06 , hc =&gt; 2.00E-06 , hct =&gt; 0.00E+00 , cmos =&gt; 1.00E-05),</v>
+        <f>ssxlibx2!A10 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L10*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L10*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L10*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L10*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L10*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L10*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L10*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L10*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L10*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L10*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L10*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L10*nA,"0.00E+00")&amp;"),"</f>
+        <v>inverter =&gt;( ssxlib =&gt; 483E-12, sxlib =&gt;  483E-12 , vxlib =&gt; 550E-12 , vsclib =&gt; 400E-12 , wsclib =&gt; 400E-12 , vgalib =&gt; 425E-12 , rgalib =&gt; 458E-12 , ac =&gt; 200E-08 , act =&gt; 400E-08 , hc =&gt; 200E-08 , hct =&gt; 0.000E+00 , cmos =&gt; 001E-08),</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" s="20" t="str">
-        <f>ssxlibx2!A11 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L11*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L11*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L11*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L11*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L11*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L11*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L11*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L11*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L11*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L11*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L11*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L11*uA,"0.00E+00")&amp;"),"</f>
-        <v>and2 =&gt;( ssxlib =&gt; 9.67E-10, sxlib =&gt;  9.67E-10 , vxlib =&gt; 1.23E-09 , vsclib =&gt; 8.92E-10 , wsclib =&gt; 8.92E-10 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 2.00E-06 , act =&gt; 4.00E-06 , hc =&gt; 2.00E-06 , hct =&gt; 0.00E+00 , cmos =&gt; 4.00E-06),</v>
+        <f>ssxlibx2!A11 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L11*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L11*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L11*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L11*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L11*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L11*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L11*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L11*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L11*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L11*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L11*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L11*nA,"0.00E+00")&amp;"),"</f>
+        <v>and2 =&gt;( ssxlib =&gt; 967E-12, sxlib =&gt;  967E-12 , vxlib =&gt; 1.233E-12 , vsclib =&gt; 892E-12 , wsclib =&gt; 892E-12 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 200E-08 , act =&gt; 400E-08 , hc =&gt; 200E-08 , hct =&gt; 0.000E+00 , cmos =&gt; 4.000E-12),</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" s="20" t="str">
-        <f>ssxlibx2!A12 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L12*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L12*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L12*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L12*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L12*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L12*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L12*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L12*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L12*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L12*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L12*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L12*uA,"0.00E+00")&amp;"),"</f>
-        <v>and3 =&gt;( ssxlib =&gt; 1.35E-09, sxlib =&gt;  1.35E-09 , vxlib =&gt; 1.48E-09 , vsclib =&gt; 1.06E-09 , wsclib =&gt; 1.06E-09 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 1.00E-05),</v>
+        <f>ssxlibx2!A12 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L12*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L12*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L12*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L12*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L12*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L12*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L12*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L12*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L12*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L12*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L12*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L12*nA,"0.00E+00")&amp;"),"</f>
+        <v>and3 =&gt;( ssxlib =&gt; 1.350E-12, sxlib =&gt;  1.350E-12 , vxlib =&gt; 1.475E-12 , vsclib =&gt; 1.058E-12 , wsclib =&gt; 1.058E-12 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 001E-08),</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" s="20" t="str">
-        <f>ssxlibx2!A13 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L13*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L13*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L13*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L13*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L13*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L13*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L13*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L13*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L13*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L13*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L13*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L13*uA,"0.00E+00")&amp;"),"</f>
-        <v>and4 =&gt;( ssxlib =&gt; 1.54E-09, sxlib =&gt;  1.54E-09 , vxlib =&gt; 1.51E-09 , vsclib =&gt; 1.25E-09 , wsclib =&gt; 1.25E-09 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 1.00E-05),</v>
+        <f>ssxlibx2!A13 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L13*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L13*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L13*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L13*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L13*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L13*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L13*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L13*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L13*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L13*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L13*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L13*nA,"0.00E+00")&amp;"),"</f>
+        <v>and4 =&gt;( ssxlib =&gt; 1.542E-12, sxlib =&gt;  1.542E-12 , vxlib =&gt; 1.508E-12 , vsclib =&gt; 1.250E-12 , wsclib =&gt; 1.250E-12 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 001E-08),</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" s="20" t="str">
-        <f>ssxlibx2!A14 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L14*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L14*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L14*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L14*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L14*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L14*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L14*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L14*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L14*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L14*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L14*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L14*uA,"0.00E+00")&amp;"),"</f>
-        <v>or2 =&gt;( ssxlib =&gt; 1.06E-09, sxlib =&gt;  1.06E-09 , vxlib =&gt; 6.83E-10 , vsclib =&gt; 8.25E-10 , wsclib =&gt; 8.25E-10 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 2.00E-06 , act =&gt; 4.00E-06 , hc =&gt; 2.00E-06 , hct =&gt; 0.00E+00 , cmos =&gt; 4.00E-06),</v>
+        <f>ssxlibx2!A14 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L14*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L14*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L14*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L14*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L14*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L14*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L14*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L14*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L14*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L14*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L14*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L14*nA,"0.00E+00")&amp;"),"</f>
+        <v>or2 =&gt;( ssxlib =&gt; 1.058E-12, sxlib =&gt;  1.058E-12 , vxlib =&gt; 683E-12 , vsclib =&gt; 825E-12 , wsclib =&gt; 825E-12 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 200E-08 , act =&gt; 400E-08 , hc =&gt; 200E-08 , hct =&gt; 0.000E+00 , cmos =&gt; 4.000E-12),</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" s="20" t="str">
-        <f>ssxlibx2!A15 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L15*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L15*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L15*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L15*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L15*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L15*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L15*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L15*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L15*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L15*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L15*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L15*uA,"0.00E+00")&amp;"),"</f>
-        <v>or3 =&gt;( ssxlib =&gt; 1.16E-09, sxlib =&gt;  1.16E-09 , vxlib =&gt; 8.50E-10 , vsclib =&gt; 1.05E-09 , wsclib =&gt; 1.05E-09 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 1.00E-05),</v>
+        <f>ssxlibx2!A15 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L15*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L15*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L15*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L15*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L15*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L15*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L15*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L15*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L15*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L15*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L15*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L15*nA,"0.00E+00")&amp;"),"</f>
+        <v>or3 =&gt;( ssxlib =&gt; 1.158E-12, sxlib =&gt;  1.158E-12 , vxlib =&gt; 850E-12 , vsclib =&gt; 1.050E-12 , wsclib =&gt; 1.050E-12 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 001E-08),</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" s="20" t="str">
-        <f>ssxlibx2!A16 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L16*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L16*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L16*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L16*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L16*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L16*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L16*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L16*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L16*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L16*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L16*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L16*uA,"0.00E+00")&amp;"),"</f>
-        <v>or4 =&gt;( ssxlib =&gt; 1.25E-09, sxlib =&gt;  1.25E-09 , vxlib =&gt; 8.92E-10 , vsclib =&gt; 1.13E-09 , wsclib =&gt; 1.13E-09 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 2.50E-04),</v>
+        <f>ssxlibx2!A16 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L16*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L16*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L16*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L16*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L16*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L16*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L16*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L16*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L16*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L16*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L16*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L16*nA,"0.00E+00")&amp;"),"</f>
+        <v>or4 =&gt;( ssxlib =&gt; 1.250E-12, sxlib =&gt;  1.250E-12 , vxlib =&gt; 892E-12 , vsclib =&gt; 1.133E-12 , wsclib =&gt; 1.133E-12 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 025E-08),</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="20" t="str">
-        <f>ssxlibx2!A17 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L17*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L17*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L17*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L17*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L17*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L17*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L17*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L17*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L17*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L17*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L17*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L17*uA,"0.00E+00")&amp;"),"</f>
-        <v>nand2 =&gt;( ssxlib =&gt; 5.75E-10, sxlib =&gt;  5.75E-10 , vxlib =&gt; 1.07E-09 , vsclib =&gt; 6.58E-10 , wsclib =&gt; 6.58E-10 , vgalib =&gt; 6.75E-10 , rgalib =&gt; 7.33E-10 , ac =&gt; 2.00E-06 , act =&gt; 2.00E-06 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 4.00E-06),</v>
+        <f>ssxlibx2!A17 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L17*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L17*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L17*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L17*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L17*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L17*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L17*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L17*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L17*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L17*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L17*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L17*nA,"0.00E+00")&amp;"),"</f>
+        <v>nand2 =&gt;( ssxlib =&gt; 575E-12, sxlib =&gt;  575E-12 , vxlib =&gt; 1.067E-12 , vsclib =&gt; 658E-12 , wsclib =&gt; 658E-12 , vgalib =&gt; 675E-12 , rgalib =&gt; 733E-12 , ac =&gt; 200E-08 , act =&gt; 200E-08 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 4.000E-12),</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="20" t="str">
-        <f>ssxlibx2!A18 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L18*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L18*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L18*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L18*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L18*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L18*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L18*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L18*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L18*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L18*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L18*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L18*uA,"0.00E+00")&amp;"),"</f>
-        <v>nand3 =&gt;( ssxlib =&gt; 7.67E-10, sxlib =&gt;  7.67E-10 , vxlib =&gt; 1.27E-09 , vsclib =&gt; 1.08E-09 , wsclib =&gt; 1.08E-09 , vgalib =&gt; 9.25E-10 , rgalib =&gt; 1.00E-09 , ac =&gt; 2.00E-06 , act =&gt; 4.00E-06 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 4.00E-06),</v>
+        <f>ssxlibx2!A18 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L18*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L18*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L18*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L18*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L18*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L18*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L18*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L18*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L18*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L18*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L18*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L18*nA,"0.00E+00")&amp;"),"</f>
+        <v>nand3 =&gt;( ssxlib =&gt; 767E-12, sxlib =&gt;  767E-12 , vxlib =&gt; 1.267E-12 , vsclib =&gt; 1.075E-12 , wsclib =&gt; 1.075E-12 , vgalib =&gt; 925E-12 , rgalib =&gt; 1.000E-12 , ac =&gt; 200E-08 , act =&gt; 400E-08 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 4.000E-12),</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="20" t="str">
-        <f>ssxlibx2!A19 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L19*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L19*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L19*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L19*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L19*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L19*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L19*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L19*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L19*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L19*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L19*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L19*uA,"0.00E+00")&amp;"),"</f>
-        <v>nand4 =&gt;( ssxlib =&gt; 9.67E-10, sxlib =&gt;  9.67E-10 , vxlib =&gt; 1.94E-09 , vsclib =&gt; 1.25E-09 , wsclib =&gt; 1.25E-09 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 2.00E-06 , act =&gt; 4.00E-06 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 5.00E-06),</v>
+        <f>ssxlibx2!A19 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L19*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L19*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L19*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L19*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L19*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L19*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L19*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L19*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L19*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L19*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L19*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L19*nA,"0.00E+00")&amp;"),"</f>
+        <v>nand4 =&gt;( ssxlib =&gt; 967E-12, sxlib =&gt;  967E-12 , vxlib =&gt; 1.942E-12 , vsclib =&gt; 1.250E-12 , wsclib =&gt; 1.250E-12 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 200E-08 , act =&gt; 400E-08 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 5.000E-12),</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="20" t="str">
-        <f>ssxlibx2!A20 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L20*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L20*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L20*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L20*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L20*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L20*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L20*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L20*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L20*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L20*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L20*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L20*uA,"0.00E+00")&amp;"),"</f>
-        <v>nor2 =&gt;( ssxlib =&gt; 5.75E-10, sxlib =&gt;  5.75E-10 , vxlib =&gt; 1.16E-09 , vsclib =&gt; 8.08E-10 , wsclib =&gt; 8.08E-10 , vgalib =&gt; 6.75E-10 , rgalib =&gt; 1.31E-09 , ac =&gt; 2.00E-06 , act =&gt; 4.00E-06 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 4.00E-06),</v>
+        <f>ssxlibx2!A20 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L20*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L20*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L20*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L20*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L20*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L20*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L20*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L20*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L20*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L20*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L20*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L20*nA,"0.00E+00")&amp;"),"</f>
+        <v>nor2 =&gt;( ssxlib =&gt; 575E-12, sxlib =&gt;  575E-12 , vxlib =&gt; 1.158E-12 , vsclib =&gt; 808E-12 , wsclib =&gt; 808E-12 , vgalib =&gt; 675E-12 , rgalib =&gt; 1.308E-12 , ac =&gt; 200E-08 , act =&gt; 400E-08 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 4.000E-12),</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" s="20" t="str">
-        <f>ssxlibx2!A21 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L21*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L21*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L21*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L21*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L21*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L21*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L21*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L21*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L21*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L21*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L21*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L21*uA,"0.00E+00")&amp;"),"</f>
-        <v>nor3 =&gt;( ssxlib =&gt; 6.75E-10, sxlib =&gt;  6.75E-10 , vxlib =&gt; 1.18E-09 , vsclib =&gt; 1.22E-09 , wsclib =&gt; 1.22E-09 , vgalib =&gt; 1.69E-09 , rgalib =&gt; 1.69E-09 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 5.00E-06),</v>
+        <f>ssxlibx2!A21 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L21*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L21*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L21*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L21*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L21*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L21*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L21*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L21*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L21*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L21*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L21*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L21*nA,"0.00E+00")&amp;"),"</f>
+        <v>nor3 =&gt;( ssxlib =&gt; 675E-12, sxlib =&gt;  675E-12 , vxlib =&gt; 1.183E-12 , vsclib =&gt; 1.217E-12 , wsclib =&gt; 1.217E-12 , vgalib =&gt; 1.692E-12 , rgalib =&gt; 1.692E-12 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 5.000E-12),</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="20" t="str">
-        <f>ssxlibx2!A22 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L22*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L22*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L22*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L22*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L22*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L22*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L22*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L22*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L22*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L22*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L22*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L22*uA,"0.00E+00")&amp;"),"</f>
-        <v>nor4 =&gt;( ssxlib =&gt; 7.67E-10, sxlib =&gt;  7.67E-10 , vxlib =&gt; 1.18E-09 , vsclib =&gt; 1.18E-09 , wsclib =&gt; 1.18E-09 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 5.00E-06),</v>
+        <f>ssxlibx2!A22 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L22*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L22*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L22*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L22*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L22*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L22*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L22*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L22*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L22*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L22*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L22*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L22*nA,"0.00E+00")&amp;"),"</f>
+        <v>nor4 =&gt;( ssxlib =&gt; 767E-12, sxlib =&gt;  767E-12 , vxlib =&gt; 1.175E-12 , vsclib =&gt; 1.183E-12 , wsclib =&gt; 1.183E-12 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 5.000E-12),</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" s="20" t="str">
-        <f>ssxlibx2!A23 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L23*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L23*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L23*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L23*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L23*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L23*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L23*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L23*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L23*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L23*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L23*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L23*uA,"0.00E+00")&amp;"),"</f>
-        <v>xor2 =&gt;( ssxlib =&gt; 1.73E-09, sxlib =&gt;  1.73E-09 , vxlib =&gt; 1.06E-09 , vsclib =&gt; 1.52E-09 , wsclib =&gt; 1.52E-09 , vgalib =&gt; 1.02E-09 , rgalib =&gt; 1.38E-09 , ac =&gt; 2.00E-06 , act =&gt; 2.00E-06 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 5.00E-05),</v>
+        <f>ssxlibx2!A23 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L23*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L23*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L23*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L23*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L23*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L23*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L23*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L23*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L23*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L23*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L23*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L23*nA,"0.00E+00")&amp;"),"</f>
+        <v>xor2 =&gt;( ssxlib =&gt; 1.733E-12, sxlib =&gt;  1.733E-12 , vxlib =&gt; 1.058E-12 , vsclib =&gt; 1.517E-12 , wsclib =&gt; 1.517E-12 , vgalib =&gt; 1.017E-12 , rgalib =&gt; 1.383E-12 , ac =&gt; 200E-08 , act =&gt; 200E-08 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 005E-08),</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" s="20" t="str">
-        <f>ssxlibx2!A24 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L24*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L24*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L24*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L24*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L24*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L24*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L24*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L24*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L24*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L24*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L24*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L24*uA,"0.00E+00")&amp;"),"</f>
-        <v>xnor2 =&gt;( ssxlib =&gt; 1.73E-09, sxlib =&gt;  1.73E-09 , vxlib =&gt; 1.02E-09 , vsclib =&gt; 1.63E-09 , wsclib =&gt; 1.63E-09 , vgalib =&gt; 1.10E-09 , rgalib =&gt; 1.38E-09 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 1.00E-04),</v>
+        <f>ssxlibx2!A24 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L24*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L24*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L24*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L24*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L24*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L24*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L24*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L24*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L24*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L24*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L24*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L24*nA,"0.00E+00")&amp;"),"</f>
+        <v>xnor2 =&gt;( ssxlib =&gt; 1.733E-12, sxlib =&gt;  1.733E-12 , vxlib =&gt; 1.017E-12 , vsclib =&gt; 1.633E-12 , wsclib =&gt; 1.633E-12 , vgalib =&gt; 1.100E-12 , rgalib =&gt; 1.383E-12 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 010E-08),</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" s="20" t="str">
-        <f>ssxlibx2!A25 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L25*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L25*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L25*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L25*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L25*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L25*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L25*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L25*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L25*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L25*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L25*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L25*uA,"0.00E+00")&amp;"),"</f>
-        <v>mux2 =&gt;( ssxlib =&gt; 1.44E-09, sxlib =&gt;  1.44E-09 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 8.58E-10 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <f>ssxlibx2!A25 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L25*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L25*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L25*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L25*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L25*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L25*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L25*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L25*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L25*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L25*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L25*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L25*nA,"0.00E+00")&amp;"),"</f>
+        <v>mux2 =&gt;( ssxlib =&gt; 1.442E-12, sxlib =&gt;  1.442E-12 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 858E-12 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" s="20" t="str">
-        <f>ssxlibx2!A26 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L26*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L26*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L26*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L26*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L26*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L26*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L26*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L26*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L26*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L26*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L26*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L26*uA,"0.00E+00")&amp;"),"</f>
-        <v>mux4 =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 8.00E-06 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <f>ssxlibx2!A26 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L26*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L26*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L26*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L26*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L26*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L26*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L26*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L26*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L26*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L26*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L26*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L26*nA,"0.00E+00")&amp;"),"</f>
+        <v>mux4 =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 800E-08 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" s="20" t="str">
-        <f>ssxlibx2!A27 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L27*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L27*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L27*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L27*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L27*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L27*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L27*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L27*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L27*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L27*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L27*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L27*uA,"0.00E+00")&amp;"),"</f>
-        <v>num163 =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 8.00E-06 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <f>ssxlibx2!A27 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L27*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L27*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L27*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L27*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L27*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L27*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L27*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L27*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L27*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L27*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L27*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L27*nA,"0.00E+00")&amp;"),"</f>
+        <v>num163 =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 800E-08 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" s="20" t="str">
-        <f>ssxlibx2!A28 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L28*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L28*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L28*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L28*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L28*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L28*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L28*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L28*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L28*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L28*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L28*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L28*uA,"0.00E+00")&amp;"),"</f>
-        <v>dff_rising_edge =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 1.77E-09 , wsclib =&gt; 1.77E-09 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <f>ssxlibx2!A28 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!L28*nA,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!L28*nA,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!L28*nA,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!L28*nA, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!L28*nA, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!L28*nA, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!L28*nA, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!L28*uA, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!L28*uA, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!L28*uA, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!L28*uA, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!L28*nA,"0.00E+00")&amp;"),"</f>
+        <v>dff_rising_edge =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 1.767E-12 , wsclib =&gt; 1.767E-12 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
       </c>
     </row>
   </sheetData>
@@ -6266,7 +6266,7 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8:L28"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7675,8 +7675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40EC2ACA-1533-4922-94A4-1C2062C36F9B}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10477,7 +10477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B16F2BC-9B4C-4AD0-9117-267F85A79AE3}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added new example to PELib: FSM2. It contains a 4 bit state machine and it's power consuption optimization using clock gating.
</commit_message>
<xml_diff>
--- a/src/PELib/gates.xlsx
+++ b/src/PELib/gates.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055D6724-4EE2-4B15-9A92-41D1A1BB8C8C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7ECA0266-3A64-4F89-8E6D-8D6A123A7F99}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="19560" windowHeight="8130" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="19560" windowHeight="8130" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="17" r:id="rId1"/>
@@ -4523,8 +4523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F873900-F695-4C83-85AF-B7B87EDD7FCF}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4925,10 +4925,10 @@
         <v>0</v>
       </c>
       <c r="M28" s="10">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="N28" s="10">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="Q28" s="10">
         <v>0</v>
@@ -4946,8 +4946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E3FCF2-1EFF-46E6-81A7-08A9A539DC92}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5297,10 +5297,10 @@
         <v>0</v>
       </c>
       <c r="M25" s="10">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="N25" s="10">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="Q25" s="10">
         <v>0</v>
@@ -5314,10 +5314,10 @@
         <v>0</v>
       </c>
       <c r="M26" s="10">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N26" s="10">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="Q26" s="10">
         <v>0</v>
@@ -5348,10 +5348,10 @@
         <v>0</v>
       </c>
       <c r="M28" s="10">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="N28" s="10">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="Q28" s="10">
         <v>0</v>
@@ -5922,13 +5922,13 @@
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" t="str">
         <f>ssxlibx2!A25 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M25*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M25*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M25*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M25*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M25*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M25*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M25*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M25*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M25*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M25*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M25*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M25*pF,"0.00E+00")&amp;"),"</f>
-        <v>mux2 =&gt;( ssxlib =&gt; 2.29E-14, sxlib =&gt;  2.38E-14 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 1.51E-14 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>mux2 =&gt;( ssxlib =&gt; 2.29E-14, sxlib =&gt;  2.38E-14 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 1.51E-14 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 7.00E-11 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" t="str">
         <f>ssxlibx2!A26 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M26*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M26*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M26*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M26*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M26*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M26*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M26*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M26*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M26*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M26*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M26*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M26*pF,"0.00E+00")&amp;"),"</f>
-        <v>mux4 =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 4.00E-11 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>mux4 =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 4.00E-11 , hct =&gt; 3.00E-11 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
@@ -5940,7 +5940,7 @@
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" t="str">
         <f>ssxlibx2!A28 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M28*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M28*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M28*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M28*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M28*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M28*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M28*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M28*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M28*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M28*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M28*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M28*pF,"0.00E+00")&amp;"),"</f>
-        <v>dff_rising_edge =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 9.31E-15 , wsclib =&gt; 9.31E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>dff_rising_edge =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 9.31E-15 , wsclib =&gt; 9.31E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 2.40E-11 , hct =&gt; 2.40E-11 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
   </sheetData>
@@ -6073,13 +6073,13 @@
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" t="str">
         <f>ssxlibx2!A25 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N25*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N25*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N25*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N25*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N25*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N25*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N25*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N25*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N25*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N25*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N25*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N25*pF,"0.00E+00")&amp;"),"</f>
-        <v>mux2 =&gt;( ssxlib =&gt; 3.50E-15, sxlib =&gt;  3.70E-15 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 4.30E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>mux2 =&gt;( ssxlib =&gt; 3.50E-15, sxlib =&gt;  3.70E-15 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 4.30E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 3.50E-12 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" t="str">
         <f>ssxlibx2!A26 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N26*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N26*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N26*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N26*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N26*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N26*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N26*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N26*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N26*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N26*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N26*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N26*pF,"0.00E+00")&amp;"),"</f>
-        <v>mux4 =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 3.50E-12 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>mux4 =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 3.50E-12 , hct =&gt; 3.50E-12 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
@@ -6091,7 +6091,7 @@
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" t="str">
         <f>ssxlibx2!A28 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N28*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N28*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N28*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N28*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N28*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N28*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N28*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N28*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N28*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N28*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N28*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N28*pF,"0.00E+00")&amp;"),"</f>
-        <v>dff_rising_edge =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 2.30E-15 , wsclib =&gt; 2.30E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>dff_rising_edge =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 2.30E-15 , wsclib =&gt; 2.30E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 3.50E-12 , hct =&gt; 3.50E-12 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
   </sheetData>
@@ -6104,7 +6104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3F6050-3A70-4B3E-887E-AAD3792C60E7}">
   <dimension ref="A2:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -6265,8 +6265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7675,8 +7675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40EC2ACA-1533-4922-94A4-1C2062C36F9B}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
FSM2 simulation files working; optimized FSM consumes more then unoptimized one; have to investigate+
</commit_message>
<xml_diff>
--- a/src/PELib/gates.xlsx
+++ b/src/PELib/gates.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7ECA0266-3A64-4F89-8E6D-8D6A123A7F99}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1B976959-5E52-4B44-A420-677C40EFC9A1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="19560" windowHeight="8130" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="19560" windowHeight="8130" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="17" r:id="rId1"/>
@@ -4524,7 +4524,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4653,10 +4653,10 @@
         <v>0</v>
       </c>
       <c r="M12" s="10">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N12" s="10">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="Q12" s="10">
         <v>0</v>
@@ -4670,10 +4670,10 @@
         <v>0</v>
       </c>
       <c r="M13" s="10">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="N13" s="10">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="Q13" s="10">
         <v>0</v>
@@ -4704,10 +4704,10 @@
         <v>0</v>
       </c>
       <c r="M15" s="10">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="N15" s="10">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="Q15" s="10">
         <v>0</v>
@@ -4721,10 +4721,10 @@
         <v>0</v>
       </c>
       <c r="M16" s="10">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="N16" s="10">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="Q16" s="10">
         <v>0</v>
@@ -4874,10 +4874,10 @@
         <v>0</v>
       </c>
       <c r="M25" s="10">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="N25" s="10">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="Q25" s="10">
         <v>0</v>
@@ -4946,8 +4946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E3FCF2-1EFF-46E6-81A7-08A9A539DC92}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5792,8 +5792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD808CF-F54B-4045-9653-9E9B5A90ECEB}">
   <dimension ref="A2:C28"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5844,13 +5844,13 @@
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="str">
         <f>ssxlibx2!A12 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M12*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M12*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M12*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M12*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M12*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M12*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M12*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M12*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M12*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M12*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M12*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M12*pF,"0.00E+00")&amp;"),"</f>
-        <v>and3 =&gt;( ssxlib =&gt; 2.66E-14, sxlib =&gt;  2.69E-14 , vxlib =&gt; 2.24E-14 , vsclib =&gt; 1.63E-14 , wsclib =&gt; 1.63E-14 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>and3 =&gt;( ssxlib =&gt; 2.66E-14, sxlib =&gt;  2.69E-14 , vxlib =&gt; 2.24E-14 , vsclib =&gt; 1.63E-14 , wsclib =&gt; 1.63E-14 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 1.80E-11 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="str">
         <f>ssxlibx2!A13 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M13*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M13*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M13*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M13*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M13*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M13*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M13*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M13*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M13*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M13*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M13*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M13*pF,"0.00E+00")&amp;"),"</f>
-        <v>and4 =&gt;( ssxlib =&gt; 2.26E-14, sxlib =&gt;  2.30E-14 , vxlib =&gt; 2.41E-14 , vsclib =&gt; 1.71E-14 , wsclib =&gt; 1.71E-14 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>and4 =&gt;( ssxlib =&gt; 2.26E-14, sxlib =&gt;  2.30E-14 , vxlib =&gt; 2.41E-14 , vsclib =&gt; 1.71E-14 , wsclib =&gt; 1.71E-14 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 1.50E-11 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5862,13 +5862,13 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" t="str">
         <f>ssxlibx2!A15 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M15*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M15*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M15*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M15*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M15*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M15*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M15*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M15*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M15*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M15*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M15*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M15*pF,"0.00E+00")&amp;"),"</f>
-        <v>or3 =&gt;( ssxlib =&gt; 2.13E-14, sxlib =&gt;  2.13E-14 , vxlib =&gt; 1.43E-14 , vsclib =&gt; 1.62E-14 , wsclib =&gt; 1.62E-14 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>or3 =&gt;( ssxlib =&gt; 2.13E-14, sxlib =&gt;  2.13E-14 , vxlib =&gt; 1.43E-14 , vsclib =&gt; 1.62E-14 , wsclib =&gt; 1.62E-14 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 2.80E-11 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" t="str">
         <f>ssxlibx2!A16 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M16*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M16*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M16*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M16*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M16*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M16*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M16*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M16*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M16*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M16*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M16*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M16*pF,"0.00E+00")&amp;"),"</f>
-        <v>or4 =&gt;( ssxlib =&gt; 2.19E-14, sxlib =&gt;  2.19E-14 , vxlib =&gt; 1.44E-14 , vsclib =&gt; 1.72E-14 , wsclib =&gt; 1.72E-14 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>or4 =&gt;( ssxlib =&gt; 2.19E-14, sxlib =&gt;  2.19E-14 , vxlib =&gt; 1.44E-14 , vsclib =&gt; 1.72E-14 , wsclib =&gt; 1.72E-14 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 1.50E-11 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
@@ -5922,7 +5922,7 @@
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" t="str">
         <f>ssxlibx2!A25 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!M25*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!M25*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!M25*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!M25*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!M25*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!M25*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!M25*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!M25*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!M25*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!M25*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!M25*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!M25*pF,"0.00E+00")&amp;"),"</f>
-        <v>mux2 =&gt;( ssxlib =&gt; 2.29E-14, sxlib =&gt;  2.38E-14 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 1.51E-14 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 7.00E-11 , cmos =&gt; 0.00E+00),</v>
+        <v>mux2 =&gt;( ssxlib =&gt; 2.29E-14, sxlib =&gt;  2.38E-14 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 1.51E-14 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 7.00E-11 , hct =&gt; 7.00E-11 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
@@ -5954,7 +5954,7 @@
   <dimension ref="B2:C28"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B8" sqref="A8:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5971,7 +5971,7 @@
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C8" t="str">
         <f>ssxlibx2!A8 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N8*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N8*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N8*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N8*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N8*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N8*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N8*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N8*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N8*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N8*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N8*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N8*pF,"0.00E+00")&amp;"),"</f>
-        <v>tristate_buffer =&gt;( ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 004E-12 , act =&gt; 004E-12 , hc =&gt; 010E-12 , hct =&gt; 004E-12 , cmos =&gt; 0.000E+00),</v>
+        <v>tristate_buffer =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 4.00E-12 , act =&gt; 4.00E-12 , hc =&gt; 1.00E-11 , hct =&gt; 3.50E-12 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
@@ -5995,13 +5995,13 @@
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C12" t="str">
         <f>ssxlibx2!A12 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N12*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N12*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N12*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N12*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N12*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N12*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N12*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N12*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N12*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N12*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N12*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N12*pF,"0.00E+00")&amp;"),"</f>
-        <v>and3 =&gt;( ssxlib =&gt; 4.90E-15, sxlib =&gt;  4.90E-15 , vxlib =&gt; 5.70E-15 , vsclib =&gt; 4.10E-15 , wsclib =&gt; 4.10E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 5.00E-12),</v>
+        <v>and3 =&gt;( ssxlib =&gt; 4.90E-15, sxlib =&gt;  4.90E-15 , vxlib =&gt; 5.70E-15 , vsclib =&gt; 4.10E-15 , wsclib =&gt; 4.10E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 3.50E-12 , hct =&gt; 0.00E+00 , cmos =&gt; 5.00E-12),</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C13" t="str">
         <f>ssxlibx2!A13 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N13*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N13*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N13*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N13*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N13*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N13*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N13*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N13*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N13*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N13*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N13*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N13*pF,"0.00E+00")&amp;"),"</f>
-        <v>and4 =&gt;( ssxlib =&gt; 4.70E-15, sxlib =&gt;  4.80E-15 , vxlib =&gt; 5.90E-15 , vsclib =&gt; 4.60E-15 , wsclib =&gt; 4.60E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>and4 =&gt;( ssxlib =&gt; 4.70E-15, sxlib =&gt;  4.80E-15 , vxlib =&gt; 5.90E-15 , vsclib =&gt; 4.60E-15 , wsclib =&gt; 4.60E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 3.50E-12 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
@@ -6013,13 +6013,13 @@
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C15" t="str">
         <f>ssxlibx2!A15 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N15*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N15*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N15*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N15*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N15*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N15*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N15*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N15*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N15*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N15*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N15*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N15*pF,"0.00E+00")&amp;"),"</f>
-        <v>or3 =&gt;( ssxlib =&gt; 4.40E-15, sxlib =&gt;  4.40E-15 , vxlib =&gt; 5.00E-15 , vsclib =&gt; 5.60E-15 , wsclib =&gt; 5.60E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 5.00E-12),</v>
+        <v>or3 =&gt;( ssxlib =&gt; 4.40E-15, sxlib =&gt;  4.40E-15 , vxlib =&gt; 5.00E-15 , vsclib =&gt; 5.60E-15 , wsclib =&gt; 5.60E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 3.50E-12 , hct =&gt; 0.00E+00 , cmos =&gt; 5.00E-12),</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C16" t="str">
         <f>ssxlibx2!A16 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N16*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N16*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N16*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N16*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N16*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N16*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N16*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N16*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N16*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N16*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N16*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N16*pF,"0.00E+00")&amp;"),"</f>
-        <v>or4 =&gt;( ssxlib =&gt; 4.20E-15, sxlib =&gt;  4.20E-15 , vxlib =&gt; 4.90E-15 , vsclib =&gt; 6.10E-15 , wsclib =&gt; 6.10E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 7.50E-12),</v>
+        <v>or4 =&gt;( ssxlib =&gt; 4.20E-15, sxlib =&gt;  4.20E-15 , vxlib =&gt; 4.90E-15 , vsclib =&gt; 6.10E-15 , wsclib =&gt; 6.10E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 3.50E-12 , hct =&gt; 0.00E+00 , cmos =&gt; 7.50E-12),</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
@@ -6073,7 +6073,7 @@
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" t="str">
         <f>ssxlibx2!A25 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!N25*fF,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!N25*fF,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!N25*fF,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!N25*fF, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!N25*fF, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!N25*fF, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!N25*fF, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!N25*pF, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!N25*pF, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!N25*pF, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!N25*pF, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!N25*pF,"0.00E+00")&amp;"),"</f>
-        <v>mux2 =&gt;( ssxlib =&gt; 3.50E-15, sxlib =&gt;  3.70E-15 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 4.30E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 3.50E-12 , cmos =&gt; 0.00E+00),</v>
+        <v>mux2 =&gt;( ssxlib =&gt; 3.50E-15, sxlib =&gt;  3.70E-15 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 4.30E-15 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 3.50E-12 , hct =&gt; 3.50E-12 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
@@ -6105,7 +6105,7 @@
   <dimension ref="A2:C28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updates to FSM2; am adauguat arii pentru familia HC in felul urmator, daca un pachet contine 4 porti logice, atunci aria ocupata am egalat cu 1/4; deci numarul portilor per pachet
</commit_message>
<xml_diff>
--- a/src/PELib/gates.xlsx
+++ b/src/PELib/gates.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1B976959-5E52-4B44-A420-677C40EFC9A1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E81C291B-2EAF-4519-B2AA-26BD4D407A46}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="19560" windowHeight="8130" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6510" yWindow="0" windowWidth="19560" windowHeight="8130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="17" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="73">
   <si>
     <t>Type Gate</t>
   </si>
@@ -200,9 +200,6 @@
   </si>
   <si>
     <t>nand2</t>
-  </si>
-  <si>
-    <t>anad3</t>
   </si>
   <si>
     <t>nand4</t>
@@ -715,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A982735-C675-46F5-98D6-7FE0AAC31E76}">
   <dimension ref="A2:C28"/>
   <sheetViews>
-    <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +724,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="21">
         <v>1E-3</v>
@@ -735,16 +732,17 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="21">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
+    <row r="7" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="str">
-        <f>ssxlibx2!A8 &amp; " =&gt;( C7ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q8*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q8*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q8*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q8*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q8*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q8*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q8*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q8*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q8*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q8*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q8*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q8*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>tristate_buffer =&gt;( C7ssxlib =&gt; 0.000E+00, sxlib =&gt;  0.000E+00 , vxlib =&gt; 0.000E+00 , vsclib =&gt; 0.000E+00 , wsclib =&gt; 0.000E+00 , vgalib =&gt; 0.000E+00 , rgalib =&gt; 0.000E+00 , ac =&gt; 0.000E+00 , act =&gt; 0.000E+00 , hc =&gt; 0.000E+00 , hct =&gt; 0.000E+00 , cmos =&gt; 0.000E+00),</v>
+        <f>ssxlibx2!A8 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q8*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q8*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q8*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q8*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q8*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q8*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q8*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q8*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q8*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q8*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q8*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q8*mm*mm,"0.00E+00")&amp;"),"</f>
+        <v>tristate_buffer =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 1.67E-07 , hct =&gt; 1.67E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -762,109 +760,109 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C11" t="str">
         <f>ssxlibx2!A11 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q11*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q11*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q11*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q11*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q11*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q11*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q11*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q11*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q11*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q11*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q11*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q11*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>and2 =&gt;( ssxlib =&gt; 1.51E-11, sxlib =&gt;  1.51E-11 , vxlib =&gt; 1.51E-11 , vsclib =&gt; 8.71E-12 , wsclib =&gt; 9.68E-12 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>and2 =&gt;( ssxlib =&gt; 1.51E-11, sxlib =&gt;  1.51E-11 , vxlib =&gt; 1.51E-11 , vsclib =&gt; 8.71E-12 , wsclib =&gt; 9.68E-12 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 2.50E-07 , hct =&gt; 2.50E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="str">
         <f>ssxlibx2!A12 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q12*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q12*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q12*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q12*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q12*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q12*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q12*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q12*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q12*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q12*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q12*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q12*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>and3 =&gt;( ssxlib =&gt; 1.82E-11, sxlib =&gt;  1.82E-11 , vxlib =&gt; 1.82E-11 , vsclib =&gt; 1.22E-11 , wsclib =&gt; 1.36E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>and3 =&gt;( ssxlib =&gt; 1.82E-11, sxlib =&gt;  1.82E-11 , vxlib =&gt; 1.82E-11 , vsclib =&gt; 1.22E-11 , wsclib =&gt; 1.36E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 3.33E-07 , hct =&gt; 3.33E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="str">
         <f>ssxlibx2!A13 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q13*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q13*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q13*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q13*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q13*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q13*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q13*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q13*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q13*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q13*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q13*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q13*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>and4 =&gt;( ssxlib =&gt; 2.12E-11, sxlib =&gt;  2.12E-11 , vxlib =&gt; 2.12E-11 , vsclib =&gt; 1.39E-11 , wsclib =&gt; 1.55E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>and4 =&gt;( ssxlib =&gt; 2.12E-11, sxlib =&gt;  2.12E-11 , vxlib =&gt; 2.12E-11 , vsclib =&gt; 1.39E-11 , wsclib =&gt; 1.55E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 5.00E-07 , hct =&gt; 5.00E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="str">
         <f>ssxlibx2!A14 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q14*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q14*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q14*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q14*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q14*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q14*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q14*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q14*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q14*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q14*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q14*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q14*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>or2 =&gt;( ssxlib =&gt; 1.51E-11, sxlib =&gt;  1.51E-11 , vxlib =&gt; 1.51E-11 , vsclib =&gt; 8.71E-12 , wsclib =&gt; 9.68E-12 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>or2 =&gt;( ssxlib =&gt; 1.51E-11, sxlib =&gt;  1.51E-11 , vxlib =&gt; 1.51E-11 , vsclib =&gt; 8.71E-12 , wsclib =&gt; 9.68E-12 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 2.50E-07 , hct =&gt; 2.50E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" t="str">
         <f>ssxlibx2!A15 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q15*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q15*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q15*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q15*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q15*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q15*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q15*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q15*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q15*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q15*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q15*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q15*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>or3 =&gt;( ssxlib =&gt; 1.82E-11, sxlib =&gt;  1.82E-11 , vxlib =&gt; 1.82E-11 , vsclib =&gt; 1.57E-11 , wsclib =&gt; 1.74E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>or3 =&gt;( ssxlib =&gt; 1.82E-11, sxlib =&gt;  1.82E-11 , vxlib =&gt; 1.82E-11 , vsclib =&gt; 1.57E-11 , wsclib =&gt; 1.74E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 3.33E-07 , hct =&gt; 3.33E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C16" t="str">
         <f>ssxlibx2!A16 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q16*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q16*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q16*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q16*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q16*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q16*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q16*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q16*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q16*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q16*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q16*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q16*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>or4 =&gt;( ssxlib =&gt; 2.12E-11, sxlib =&gt;  2.12E-11 , vxlib =&gt; 2.42E-11 , vsclib =&gt; 1.92E-11 , wsclib =&gt; 2.13E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>or4 =&gt;( ssxlib =&gt; 2.12E-11, sxlib =&gt;  2.12E-11 , vxlib =&gt; 2.42E-11 , vsclib =&gt; 1.92E-11 , wsclib =&gt; 2.13E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 5.00E-07 , hct =&gt; 5.00E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="str">
         <f>ssxlibx2!A17 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q17*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q17*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q17*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q17*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q17*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q17*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q17*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q17*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q17*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q17*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q17*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q17*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>nand2 =&gt;( ssxlib =&gt; 1.21E-11, sxlib =&gt;  1.21E-11 , vxlib =&gt; 1.21E-11 , vsclib =&gt; 6.97E-12 , wsclib =&gt; 7.74E-12 , vgalib =&gt; 8.52E-12 , rgalib =&gt; 8.52E-12 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>nand2 =&gt;( ssxlib =&gt; 1.21E-11, sxlib =&gt;  1.21E-11 , vxlib =&gt; 1.21E-11 , vsclib =&gt; 6.97E-12 , wsclib =&gt; 7.74E-12 , vgalib =&gt; 8.52E-12 , rgalib =&gt; 8.52E-12 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 2.50E-07 , hct =&gt; 2.50E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="str">
         <f>ssxlibx2!A18 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q18*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q18*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q18*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q18*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q18*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q18*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q18*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q18*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q18*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q18*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q18*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q18*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>nand3 =&gt;( ssxlib =&gt; 1.51E-11, sxlib =&gt;  1.51E-11 , vxlib =&gt; 1.51E-11 , vsclib =&gt; 1.39E-11 , wsclib =&gt; 1.55E-11 , vgalib =&gt; 1.70E-11 , rgalib =&gt; 1.70E-11 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>nand3 =&gt;( ssxlib =&gt; 1.51E-11, sxlib =&gt;  1.51E-11 , vxlib =&gt; 1.51E-11 , vsclib =&gt; 1.39E-11 , wsclib =&gt; 1.55E-11 , vgalib =&gt; 1.70E-11 , rgalib =&gt; 1.70E-11 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 3.33E-07 , hct =&gt; 3.33E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" t="str">
         <f>ssxlibx2!A19 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q19*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q19*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q19*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q19*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q19*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q19*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q19*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q19*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q19*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q19*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q19*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q19*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>nand4 =&gt;( ssxlib =&gt; 1.82E-11, sxlib =&gt;  1.82E-11 , vxlib =&gt; 2.72E-11 , vsclib =&gt; 1.74E-11 , wsclib =&gt; 1.94E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>nand4 =&gt;( ssxlib =&gt; 1.82E-11, sxlib =&gt;  1.82E-11 , vxlib =&gt; 2.72E-11 , vsclib =&gt; 1.74E-11 , wsclib =&gt; 1.94E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 5.00E-07 , hct =&gt; 5.00E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" t="str">
         <f>ssxlibx2!A20 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q20*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q20*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q20*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q20*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q20*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q20*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q20*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q20*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q20*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q20*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q20*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q20*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>nor2 =&gt;( ssxlib =&gt; 1.21E-11, sxlib =&gt;  1.21E-11 , vxlib =&gt; 1.82E-11 , vsclib =&gt; 1.05E-11 , wsclib =&gt; 1.16E-11 , vgalib =&gt; 1.70E-11 , rgalib =&gt; 1.70E-11 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>nor2 =&gt;( ssxlib =&gt; 1.21E-11, sxlib =&gt;  1.21E-11 , vxlib =&gt; 1.82E-11 , vsclib =&gt; 1.05E-11 , wsclib =&gt; 1.16E-11 , vgalib =&gt; 1.70E-11 , rgalib =&gt; 1.70E-11 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 2.50E-07 , hct =&gt; 2.50E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21" t="str">
         <f>ssxlibx2!A21 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q21*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q21*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q21*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q21*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q21*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q21*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q21*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q21*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q21*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q21*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q21*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q21*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>nor3 =&gt;( ssxlib =&gt; 1.51E-11, sxlib =&gt;  1.51E-11 , vxlib =&gt; 2.12E-11 , vsclib =&gt; 1.92E-11 , wsclib =&gt; 2.13E-11 , vgalib =&gt; 2.56E-11 , rgalib =&gt; 2.56E-11 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>nor3 =&gt;( ssxlib =&gt; 1.51E-11, sxlib =&gt;  1.51E-11 , vxlib =&gt; 2.12E-11 , vsclib =&gt; 1.92E-11 , wsclib =&gt; 2.13E-11 , vgalib =&gt; 2.56E-11 , rgalib =&gt; 2.56E-11 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 3.33E-07 , hct =&gt; 3.33E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" t="str">
         <f>ssxlibx2!A22 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q22*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q22*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q22*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q22*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q22*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q22*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q22*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q22*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q22*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q22*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q22*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q22*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>nor4 =&gt;( ssxlib =&gt; 1.82E-11, sxlib =&gt;  1.82E-11 , vxlib =&gt; 2.72E-11 , vsclib =&gt; 2.44E-11 , wsclib =&gt; 2.71E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>nor4 =&gt;( ssxlib =&gt; 1.82E-11, sxlib =&gt;  1.82E-11 , vxlib =&gt; 2.72E-11 , vsclib =&gt; 2.44E-11 , wsclib =&gt; 2.71E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 5.00E-07 , hct =&gt; 5.00E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23" t="str">
         <f>ssxlibx2!A23 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q23*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q23*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q23*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q23*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q23*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q23*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q23*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q23*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q23*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q23*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q23*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q23*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>xor2 =&gt;( ssxlib =&gt; 2.72E-11, sxlib =&gt;  2.72E-11 , vxlib =&gt; 2.12E-11 , vsclib =&gt; 2.44E-11 , wsclib =&gt; 2.71E-11 , vgalib =&gt; 2.56E-11 , rgalib =&gt; 2.56E-11 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>xor2 =&gt;( ssxlib =&gt; 2.72E-11, sxlib =&gt;  2.72E-11 , vxlib =&gt; 2.12E-11 , vsclib =&gt; 2.44E-11 , wsclib =&gt; 2.71E-11 , vgalib =&gt; 2.56E-11 , rgalib =&gt; 2.56E-11 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 2.50E-07 , hct =&gt; 2.50E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24" t="str">
         <f>ssxlibx2!A24 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q24*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q24*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q24*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q24*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q24*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q24*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q24*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q24*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q24*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q24*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q24*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q24*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>xnor2 =&gt;( ssxlib =&gt; 2.72E-11, sxlib =&gt;  2.72E-11 , vxlib =&gt; 2.12E-11 , vsclib =&gt; 2.27E-11 , wsclib =&gt; 2.52E-11 , vgalib =&gt; 2.56E-11 , rgalib =&gt; 2.56E-11 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>xnor2 =&gt;( ssxlib =&gt; 2.72E-11, sxlib =&gt;  2.72E-11 , vxlib =&gt; 2.12E-11 , vsclib =&gt; 2.27E-11 , wsclib =&gt; 2.52E-11 , vgalib =&gt; 2.56E-11 , rgalib =&gt; 2.56E-11 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 2.50E-07 , hct =&gt; 2.50E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" t="str">
         <f>ssxlibx2!A25 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q25*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q25*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q25*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q25*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q25*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q25*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q25*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q25*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q25*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q25*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q25*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q25*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>mux2 =&gt;( ssxlib =&gt; 2.72E-11, sxlib =&gt;  2.72E-11 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 1.55E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>mux2 =&gt;( ssxlib =&gt; 2.72E-11, sxlib =&gt;  2.72E-11 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 1.55E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 2.50E-07 , hct =&gt; 2.50E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" t="str">
         <f>ssxlibx2!A26 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q26*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q26*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q26*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q26*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q26*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q26*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q26*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q26*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q26*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q26*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q26*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q26*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>mux4 =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>mux4 =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 5.00E-07 , hct =&gt; 5.00E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27" t="str">
         <f>ssxlibx2!A27 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q27*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q27*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q27*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q27*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q27*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q27*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q27*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q27*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q27*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q27*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q27*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q27*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>num163 =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>num163 =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 0.00E+00 , wsclib =&gt; 0.00E+00 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 1.00E-06 , hct =&gt; 1.00E-06 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28" t="str">
         <f>ssxlibx2!A28 &amp; " =&gt;( ssxlib =&gt; " &amp; TEXT(ssxlibx2!Q28*um*um,"0.00E+00") &amp; ", sxlib =&gt;  "  &amp; TEXT(sxlibx2!Q28*um*um,"0.00E+00") &amp; " , vxlib =&gt; " &amp; TEXT(vxlibx2!Q28*um*um,"0.00E+00")&amp; " , vsclib =&gt; " &amp; TEXT(vsclibx2!Q28*um*um, "0.00E+00") &amp; " , wsclib =&gt; " &amp; TEXT(wsclibx2!Q28*um*um, "0.00E+00") &amp; " , vgalib =&gt; " &amp; TEXT(vgalibx2!Q28*um*um, "0.00E+00") &amp; " , rgalib =&gt; " &amp; TEXT(rgalibx2!Q28*um*um, "0.00E+00") &amp; " , ac =&gt; " &amp; TEXT(ac!Q28*mm*mm, "0.00E+00") &amp; " , act =&gt; " &amp; TEXT(act!Q28*mm*mm, "0.00E+00") &amp; " , hc =&gt; " &amp; TEXT(hc!Q28*mm*mm, "0.00E+00") &amp; " , hct =&gt; " &amp; TEXT(hct!Q28*mm*mm, "0.00E+00") &amp; " , cmos =&gt; " &amp; TEXT(cmos!Q28*mm*mm,"0.00E+00")&amp;"),"</f>
-        <v>dff_rising_edge =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 4.36E-11 , wsclib =&gt; 3.48E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 0.00E+00 , hct =&gt; 0.00E+00 , cmos =&gt; 0.00E+00),</v>
+        <v>dff_rising_edge =&gt;( ssxlib =&gt; 0.00E+00, sxlib =&gt;  0.00E+00 , vxlib =&gt; 0.00E+00 , vsclib =&gt; 4.36E-11 , wsclib =&gt; 3.48E-11 , vgalib =&gt; 0.00E+00 , rgalib =&gt; 0.00E+00 , ac =&gt; 0.00E+00 , act =&gt; 0.00E+00 , hc =&gt; 5.00E-07 , hct =&gt; 5.00E-07 , cmos =&gt; 0.00E+00),</v>
       </c>
     </row>
   </sheetData>
@@ -1613,7 +1611,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B18">
         <v>2.7</v>
@@ -1672,7 +1670,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1731,7 +1729,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20">
         <v>2.7</v>
@@ -1790,7 +1788,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -1849,7 +1847,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1908,7 +1906,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -1967,7 +1965,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -2026,7 +2024,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -2085,7 +2083,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -2144,7 +2142,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -2203,7 +2201,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -3012,7 +3010,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B18">
         <v>2.7</v>
@@ -3071,7 +3069,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -3130,7 +3128,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20">
         <v>2.7</v>
@@ -3189,7 +3187,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>4</v>
@@ -3248,7 +3246,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -3307,7 +3305,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -3366,7 +3364,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -3425,7 +3423,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -3484,7 +3482,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -3543,7 +3541,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -3602,7 +3600,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -3903,7 +3901,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="L18" s="10">
         <v>2</v>
@@ -3920,7 +3918,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L19" s="10">
         <v>2</v>
@@ -3937,7 +3935,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L20" s="10">
         <v>2</v>
@@ -3954,7 +3952,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L21" s="10">
         <v>0</v>
@@ -3971,7 +3969,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L22" s="10">
         <v>0</v>
@@ -3988,7 +3986,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L23" s="10">
         <v>2</v>
@@ -4005,7 +4003,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L24" s="10">
         <v>0</v>
@@ -4022,7 +4020,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L25" s="10">
         <v>0</v>
@@ -4039,7 +4037,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L26" s="10">
         <v>0</v>
@@ -4056,7 +4054,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L27" s="10">
         <v>0</v>
@@ -4073,7 +4071,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L28" s="10">
         <v>0</v>
@@ -4326,7 +4324,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="L18" s="10">
         <v>4</v>
@@ -4343,7 +4341,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L19" s="10">
         <v>4</v>
@@ -4360,7 +4358,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L20" s="10">
         <v>4</v>
@@ -4377,7 +4375,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L21" s="10">
         <v>0</v>
@@ -4394,7 +4392,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L22" s="10">
         <v>0</v>
@@ -4411,7 +4409,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L23" s="10">
         <v>2</v>
@@ -4428,7 +4426,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L24" s="10">
         <v>0</v>
@@ -4445,7 +4443,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L25" s="10">
         <v>0</v>
@@ -4462,7 +4460,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L26" s="10">
         <v>0</v>
@@ -4479,7 +4477,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L27" s="10">
         <v>0</v>
@@ -4496,7 +4494,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L28" s="10">
         <v>0</v>
@@ -4523,8 +4521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F873900-F695-4C83-85AF-B7B87EDD7FCF}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8:Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4591,7 +4589,8 @@
         <v>10</v>
       </c>
       <c r="Q8" s="10">
-        <v>0</v>
+        <f>1/6</f>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -4642,7 +4641,8 @@
         <v>3.5</v>
       </c>
       <c r="Q11" s="10">
-        <v>0</v>
+        <f>1/4</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -4659,7 +4659,8 @@
         <v>3.5</v>
       </c>
       <c r="Q12" s="10">
-        <v>0</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -4676,7 +4677,8 @@
         <v>3.5</v>
       </c>
       <c r="Q13" s="10">
-        <v>0</v>
+        <f>1/2</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -4693,7 +4695,8 @@
         <v>3.5</v>
       </c>
       <c r="Q14" s="10">
-        <v>0</v>
+        <f t="shared" ref="Q14:Q19" si="0">1/4</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -4710,7 +4713,8 @@
         <v>3.5</v>
       </c>
       <c r="Q15" s="10">
-        <v>0</v>
+        <f t="shared" ref="Q15:Q19" si="1">1/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -4727,7 +4731,8 @@
         <v>3.5</v>
       </c>
       <c r="Q16" s="10">
-        <v>0</v>
+        <f t="shared" ref="Q16:Q19" si="2">1/2</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -4744,12 +4749,13 @@
         <v>3.5</v>
       </c>
       <c r="Q17" s="10">
-        <v>0</v>
+        <f t="shared" ref="Q17:Q19" si="3">1/4</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="L18" s="10">
         <v>0</v>
@@ -4761,12 +4767,13 @@
         <v>3.5</v>
       </c>
       <c r="Q18" s="10">
-        <v>0</v>
+        <f t="shared" ref="Q18:Q19" si="4">1/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L19" s="10">
         <v>0</v>
@@ -4778,12 +4785,13 @@
         <v>3.5</v>
       </c>
       <c r="Q19" s="10">
-        <v>0</v>
+        <f t="shared" ref="Q19" si="5">1/2</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L20" s="10">
         <v>0</v>
@@ -4795,12 +4803,13 @@
         <v>3.5</v>
       </c>
       <c r="Q20" s="10">
-        <v>0</v>
+        <f>1/4</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L21" s="10">
         <v>0</v>
@@ -4812,12 +4821,13 @@
         <v>0</v>
       </c>
       <c r="Q21" s="10">
-        <v>0</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L22" s="10">
         <v>0</v>
@@ -4829,12 +4839,13 @@
         <v>0</v>
       </c>
       <c r="Q22" s="10">
-        <v>0</v>
+        <f>1/2</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L23" s="10">
         <v>0</v>
@@ -4846,12 +4857,12 @@
         <v>3.5</v>
       </c>
       <c r="Q23" s="10">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L24" s="10">
         <v>0</v>
@@ -4863,12 +4874,12 @@
         <v>0</v>
       </c>
       <c r="Q24" s="10">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L25" s="10">
         <v>0</v>
@@ -4880,12 +4891,13 @@
         <v>3.5</v>
       </c>
       <c r="Q25" s="10">
-        <v>0</v>
+        <f>1/4</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L26" s="10">
         <v>8</v>
@@ -4897,12 +4909,13 @@
         <v>3.5</v>
       </c>
       <c r="Q26" s="10">
-        <v>0</v>
+        <f>1/2</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L27" s="10">
         <v>8</v>
@@ -4914,12 +4927,12 @@
         <v>3.5</v>
       </c>
       <c r="Q27" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L28" s="10">
         <v>0</v>
@@ -4931,7 +4944,8 @@
         <v>3.5</v>
       </c>
       <c r="Q28" s="10">
-        <v>0</v>
+        <f>1/2</f>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -4946,8 +4960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E3FCF2-1EFF-46E6-81A7-08A9A539DC92}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8:Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5014,7 +5028,8 @@
         <v>3.5</v>
       </c>
       <c r="Q8" s="10">
-        <v>0</v>
+        <f>1/6</f>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -5065,7 +5080,8 @@
         <v>3.5</v>
       </c>
       <c r="Q11" s="10">
-        <v>0</v>
+        <f>1/4</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -5082,7 +5098,8 @@
         <v>0</v>
       </c>
       <c r="Q12" s="10">
-        <v>0</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -5099,7 +5116,8 @@
         <v>0</v>
       </c>
       <c r="Q13" s="10">
-        <v>0</v>
+        <f>1/2</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -5116,7 +5134,8 @@
         <v>3.5</v>
       </c>
       <c r="Q14" s="10">
-        <v>0</v>
+        <f t="shared" ref="Q14:Q19" si="0">1/4</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -5133,7 +5152,8 @@
         <v>0</v>
       </c>
       <c r="Q15" s="10">
-        <v>0</v>
+        <f t="shared" ref="Q15:Q19" si="1">1/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -5150,7 +5170,8 @@
         <v>0</v>
       </c>
       <c r="Q16" s="10">
-        <v>0</v>
+        <f t="shared" ref="Q16:Q19" si="2">1/2</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -5167,12 +5188,13 @@
         <v>3.5</v>
       </c>
       <c r="Q17" s="10">
-        <v>0</v>
+        <f t="shared" ref="Q17:Q19" si="3">1/4</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="L18" s="10">
         <v>0</v>
@@ -5184,12 +5206,13 @@
         <v>3.5</v>
       </c>
       <c r="Q18" s="10">
-        <v>0</v>
+        <f t="shared" ref="Q18:Q19" si="4">1/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L19" s="10">
         <v>0</v>
@@ -5201,12 +5224,13 @@
         <v>3.5</v>
       </c>
       <c r="Q19" s="10">
-        <v>0</v>
+        <f t="shared" ref="Q19" si="5">1/2</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L20" s="10">
         <v>0</v>
@@ -5218,12 +5242,13 @@
         <v>3.5</v>
       </c>
       <c r="Q20" s="10">
-        <v>0</v>
+        <f>1/4</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L21" s="10">
         <v>0</v>
@@ -5235,12 +5260,13 @@
         <v>0</v>
       </c>
       <c r="Q21" s="10">
-        <v>0</v>
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L22" s="10">
         <v>0</v>
@@ -5252,12 +5278,13 @@
         <v>0</v>
       </c>
       <c r="Q22" s="10">
-        <v>0</v>
+        <f>1/2</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L23" s="10">
         <v>0</v>
@@ -5269,12 +5296,12 @@
         <v>3.5</v>
       </c>
       <c r="Q23" s="10">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L24" s="10">
         <v>0</v>
@@ -5286,12 +5313,12 @@
         <v>0</v>
       </c>
       <c r="Q24" s="10">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L25" s="10">
         <v>0</v>
@@ -5303,12 +5330,13 @@
         <v>3.5</v>
       </c>
       <c r="Q25" s="10">
-        <v>0</v>
+        <f>1/4</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L26" s="10">
         <v>0</v>
@@ -5320,12 +5348,13 @@
         <v>3.5</v>
       </c>
       <c r="Q26" s="10">
-        <v>0</v>
+        <f>1/2</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L27" s="10">
         <v>0</v>
@@ -5337,12 +5366,12 @@
         <v>0</v>
       </c>
       <c r="Q27" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L28" s="10">
         <v>0</v>
@@ -5354,7 +5383,8 @@
         <v>3.5</v>
       </c>
       <c r="Q28" s="10">
-        <v>0</v>
+        <f>1/2</f>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -5595,7 +5625,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="L18" s="10">
         <v>4</v>
@@ -5612,7 +5642,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L19" s="10">
         <v>5</v>
@@ -5629,7 +5659,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L20" s="10">
         <v>4</v>
@@ -5646,7 +5676,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L21" s="10">
         <v>5</v>
@@ -5663,7 +5693,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L22" s="10">
         <v>5</v>
@@ -5680,7 +5710,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L23" s="10">
         <v>50</v>
@@ -5697,7 +5727,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L24" s="10">
         <v>100</v>
@@ -5714,7 +5744,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L25" s="10">
         <v>0</v>
@@ -5731,7 +5761,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L26" s="10">
         <v>0</v>
@@ -5748,7 +5778,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L27" s="10">
         <v>0</v>
@@ -5765,7 +5795,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L28" s="10">
         <v>0</v>
@@ -5792,7 +5822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD808CF-F54B-4045-9653-9E9B5A90ECEB}">
   <dimension ref="A2:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
@@ -5803,7 +5833,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="21">
         <v>9.9999999999999998E-13</v>
@@ -5811,7 +5841,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="21">
         <v>1.0000000000000001E-15</v>
@@ -6115,7 +6145,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="21">
         <v>9.9999999999999995E-7</v>
@@ -6123,7 +6153,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="21">
         <v>1.0000000000000001E-9</v>
@@ -7006,7 +7036,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18">
         <v>1.7</v>
@@ -7065,7 +7095,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -7124,7 +7154,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20">
         <v>1.3</v>
@@ -7183,7 +7213,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>1.7</v>
@@ -7242,7 +7272,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -7301,7 +7331,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -7360,7 +7390,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -7419,7 +7449,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -7478,7 +7508,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -7537,7 +7567,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -7596,7 +7626,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -8412,7 +8442,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B18">
         <v>1.7</v>
@@ -8471,7 +8501,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19">
         <v>2</v>
@@ -8530,7 +8560,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20">
         <v>1.3</v>
@@ -8589,7 +8619,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>1.7</v>
@@ -8648,7 +8678,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -8707,7 +8737,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -8766,7 +8796,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24">
         <v>3</v>
@@ -8825,7 +8855,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -8884,7 +8914,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -8943,7 +8973,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -9002,7 +9032,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -9812,7 +9842,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B18">
         <v>1.7</v>
@@ -9871,7 +9901,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -9930,7 +9960,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -9989,7 +10019,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>2.2999999999999998</v>
@@ -10048,7 +10078,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -10107,7 +10137,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23">
         <v>2.2999999999999998</v>
@@ -10166,7 +10196,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24">
         <v>2.2999999999999998</v>
@@ -10225,7 +10255,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -10284,7 +10314,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -10343,7 +10373,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -10402,7 +10432,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -11213,7 +11243,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B18">
         <v>2.7</v>
@@ -11272,7 +11302,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19">
         <v>3.3</v>
@@ -11331,7 +11361,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -11390,7 +11420,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>3.7</v>
@@ -11449,7 +11479,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22">
         <v>4.7</v>
@@ -11508,7 +11538,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23">
         <v>4.7</v>
@@ -11567,7 +11597,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24">
         <v>4.3</v>
@@ -11626,7 +11656,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -11685,7 +11715,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -11744,7 +11774,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -11803,7 +11833,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28">
         <v>6</v>
@@ -12614,7 +12644,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B18">
         <v>2.7</v>
@@ -12673,7 +12703,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19">
         <v>3.3</v>
@@ -12732,7 +12762,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -12791,7 +12821,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>3.7</v>
@@ -12850,7 +12880,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22">
         <v>4.7</v>
@@ -12909,7 +12939,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23">
         <v>4.7</v>
@@ -12968,7 +12998,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24">
         <v>4.3</v>
@@ -13027,7 +13057,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25">
         <v>2.7</v>
@@ -13086,7 +13116,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -13145,7 +13175,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -13204,7 +13234,7 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28">
         <v>6</v>

</xml_diff>